<commit_message>
Updating instructions documents and supporting files for V1.4. Only remaining document not yet updated is Operating Procedures
</commit_message>
<xml_diff>
--- a/autorally_platform_parts_list.xlsx
+++ b/autorally_platform_parts_list.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\AutoRally_Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{545C1C6F-302F-48B1-9374-D9DE3D412012}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoRally Platform Parts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="610">
   <si>
     <t>AutoRally Platform Parts List</t>
   </si>
@@ -1428,12 +1429,6 @@
     <t>USB Isolator</t>
   </si>
   <si>
-    <t>https://www.adafruit.com/product/2107</t>
-  </si>
-  <si>
-    <t>Adafruit USB Isolator - 100mA Isolated Low/Full Speed USB</t>
-  </si>
-  <si>
     <t>Base Station</t>
   </si>
   <si>
@@ -1488,9 +1483,6 @@
     <t>https://www.pjrc.com/store/teensylc_pins.html</t>
   </si>
   <si>
-    <t>https://www.pjrc.com/store/teensy36_pins.html</t>
-  </si>
-  <si>
     <t>The base station GPS provides RTK corrections to the robot to greatly increase the position accuracy. One GPS base station can send corrections to multiple robots.</t>
   </si>
   <si>
@@ -1509,9 +1501,6 @@
     <t>https://www.amazon.com/Neiko-01408A-Electronic-Digital-Caliper/dp/B000NEA0P8/</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/vector-electronics/8029/V2025-ND/1886431</t>
-  </si>
-  <si>
     <t>Hex drivers, short</t>
   </si>
   <si>
@@ -1605,9 +1594,6 @@
     <t>Power receptacle dust cover</t>
   </si>
   <si>
-    <t>USB A to mini-B, 6 in</t>
-  </si>
-  <si>
     <t>USB 3.0 A to microB, 0.5m</t>
   </si>
   <si>
@@ -1824,18 +1810,6 @@
     <t>100' 12-conductor cable, 24 awg stranded wire</t>
   </si>
   <si>
-    <t>Breadboard, 2"x3" through hole solder</t>
-  </si>
-  <si>
-    <t>Only needed if using Teensy 3.6 in electronics box</t>
-  </si>
-  <si>
-    <t>Only needed if Arduino Due is nto available electronics box</t>
-  </si>
-  <si>
-    <t>Teensy 3.6, for electronics box</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT2K20/CF14JT2K20CT-ND/1830358</t>
   </si>
   <si>
@@ -1852,12 +1826,42 @@
   </si>
   <si>
     <t>http://www.castlecreations.com/en/pc-software-and-cables-2/castle-link-v3-usb-programming-kit-011-0119-00</t>
+  </si>
+  <si>
+    <t>USB A to B, 6 in</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/900</t>
+  </si>
+  <si>
+    <t>https://www.sealevel.com/product/iso-1-seaiso-single-port-inline-usb-isolator-ul-recognized/</t>
+  </si>
+  <si>
+    <t>Alternate Part</t>
+  </si>
+  <si>
+    <t>EMI Sheilding Textile, 1 inch width, 33 m long</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=732-10216-ND</t>
+  </si>
+  <si>
+    <t>USB A to mini-B, 6in</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/899</t>
+  </si>
+  <si>
+    <t>USB A to B, 1.5 ft</t>
+  </si>
+  <si>
+    <t>https://www.monoprice.com/product?p_id=5438</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mmmm&quot;, &quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
@@ -2139,7 +2143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -2290,6 +2294,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2882,11 +2899,11 @@
     <xf numFmtId="0" fontId="18" fillId="15" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="5" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3365,14 +3382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O346"/>
+  <dimension ref="A1:O347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A126"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183:A263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3384,7 +3401,7 @@
     <col min="6" max="6" width="10.6328125"/>
     <col min="7" max="7" width="13.1796875"/>
     <col min="8" max="8" width="104.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14"/>
+    <col min="9" max="9" width="80.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="26" width="7.26953125"/>
     <col min="27" max="1025" width="14.54296875"/>
   </cols>
@@ -3431,7 +3448,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="232" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B4" s="233"/>
       <c r="C4" s="233"/>
@@ -3443,7 +3460,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="232" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B5" s="233"/>
       <c r="C5" s="233"/>
@@ -3455,7 +3472,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="232" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B6" s="233"/>
       <c r="C6" s="233"/>
@@ -3467,7 +3484,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="239" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B7" s="240"/>
       <c r="C7" s="240"/>
@@ -3489,7 +3506,7 @@
     </row>
     <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="235" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B9" s="235"/>
       <c r="C9" s="235"/>
@@ -3524,7 +3541,7 @@
     <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="206" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -3548,7 +3565,7 @@
     <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15"/>
       <c r="B14" s="189" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="13"/>
@@ -3560,7 +3577,7 @@
     <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="20" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="13"/>
@@ -3579,7 +3596,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
       <c r="B17" s="5"/>
       <c r="C17" s="27"/>
@@ -3589,7 +3606,7 @@
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="74"/>
       <c r="B18" s="75" t="s">
         <v>3</v>
@@ -3612,8 +3629,11 @@
       <c r="H18" s="77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="224" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="236" t="s">
         <v>9</v>
       </c>
@@ -3639,7 +3659,7 @@
         <v>http://www.davesmotors.com/hpi-109964b-hpi-baja-5sc-1_5-gas-rc-short-course-truck-w_2_4-ghz-radio-black.html</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="236"/>
       <c r="B20" s="78" t="s">
         <v>305</v>
@@ -3662,7 +3682,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="236"/>
       <c r="B21" s="78" t="s">
         <v>308</v>
@@ -3685,7 +3705,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="145" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" s="145" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="236"/>
       <c r="B22" s="78" t="s">
         <v>10</v>
@@ -3709,7 +3729,7 @@
         <v>http://www.davesmotors.com/tr800</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="236"/>
       <c r="B23" s="78" t="s">
         <v>300</v>
@@ -3732,7 +3752,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="236"/>
       <c r="B24" s="78" t="s">
         <v>11</v>
@@ -3756,7 +3776,7 @@
         <v>http://www.davesmotors.com/s.nl/it.A/id.3515/.f</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="236"/>
       <c r="B25" s="78" t="s">
         <v>12</v>
@@ -3779,7 +3799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="236"/>
       <c r="B26" s="78" t="s">
         <v>14</v>
@@ -3803,7 +3823,7 @@
         <v>http://www.davesmotors.com/hostile-zero-growth-foams-hpi-baja-5t-5sc-losi-5ive-desert-buggy-xl-dbxl-HPI4817-LOSB7241-LOS45006.html</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="236"/>
       <c r="B27" s="78" t="s">
         <v>15</v>
@@ -3827,7 +3847,7 @@
         <v>http://www.davesmotors.com/hostile-zero-growth-foams-hpi-baja-5t-5sc-rear-HPI4818-4818.html</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="236"/>
       <c r="B28" s="78" t="s">
         <v>20</v>
@@ -3850,13 +3870,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="236"/>
       <c r="B29" s="78" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C29" s="79" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D29" s="80">
         <v>19.989999999999998</v>
@@ -3870,10 +3890,10 @@
       </c>
       <c r="G29" s="81"/>
       <c r="H29" s="82" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="236"/>
       <c r="B30" s="78" t="s">
         <v>16</v>
@@ -3896,7 +3916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="236"/>
       <c r="B31" s="78" t="s">
         <v>18</v>
@@ -3919,7 +3939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="236"/>
       <c r="B32" s="78" t="s">
         <v>328</v>
@@ -4159,10 +4179,10 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="236"/>
       <c r="B42" s="177" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C42" s="178" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D42" s="179">
         <v>62.99</v>
@@ -4176,7 +4196,7 @@
       </c>
       <c r="G42" s="180"/>
       <c r="H42" s="181" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -4299,10 +4319,10 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="236"/>
       <c r="B50" s="78" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C50" s="79" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D50" s="80">
         <v>7.99</v>
@@ -4316,16 +4336,16 @@
       </c>
       <c r="G50" s="81"/>
       <c r="H50" s="82" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="236"/>
       <c r="B51" s="78" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C51" s="79" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D51" s="80">
         <v>4.34</v>
@@ -4339,7 +4359,7 @@
       </c>
       <c r="G51" s="81"/>
       <c r="H51" s="82" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -4381,7 +4401,7 @@
         <v>331</v>
       </c>
       <c r="C54" s="79" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D54" s="80">
         <v>4.49</v>
@@ -4395,7 +4415,7 @@
       </c>
       <c r="G54" s="81"/>
       <c r="H54" s="149" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -4625,7 +4645,7 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="236"/>
       <c r="B67" s="78" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="C67" s="79"/>
       <c r="D67" s="80">
@@ -4640,7 +4660,7 @@
       </c>
       <c r="G67" s="81"/>
       <c r="H67" s="82" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -4769,7 +4789,7 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="236"/>
       <c r="B74" s="78" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="C74" s="79"/>
       <c r="D74" s="80">
@@ -4784,13 +4804,13 @@
       </c>
       <c r="G74" s="81"/>
       <c r="H74" s="82" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="236"/>
       <c r="B75" s="78" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="C75" s="79"/>
       <c r="D75" s="80">
@@ -4805,13 +4825,13 @@
       </c>
       <c r="G75" s="81"/>
       <c r="H75" s="82" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="236"/>
       <c r="B76" s="78" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="C76" s="79"/>
       <c r="D76" s="80">
@@ -4826,7 +4846,7 @@
       </c>
       <c r="G76" s="81"/>
       <c r="H76" s="82" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
@@ -4878,7 +4898,7 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="236"/>
       <c r="B79" s="97" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C79" s="98" t="s">
         <v>69</v>
@@ -4895,7 +4915,7 @@
       </c>
       <c r="G79" s="100"/>
       <c r="H79" s="101" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -5016,7 +5036,7 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="236"/>
       <c r="B85" s="97" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="C85" s="98" t="s">
         <v>53</v>
@@ -5033,13 +5053,13 @@
       </c>
       <c r="G85" s="100"/>
       <c r="H85" s="101" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="236"/>
       <c r="B86" s="97" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="C86" s="98" t="s">
         <v>71</v>
@@ -5056,13 +5076,13 @@
       </c>
       <c r="G86" s="100"/>
       <c r="H86" s="101" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="236"/>
       <c r="B87" s="78" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="C87" s="79" t="s">
         <v>71</v>
@@ -5079,13 +5099,13 @@
       </c>
       <c r="G87" s="81"/>
       <c r="H87" s="82" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="236"/>
       <c r="B88" s="78" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="C88" s="79" t="s">
         <v>71</v>
@@ -5102,7 +5122,7 @@
       </c>
       <c r="G88" s="81"/>
       <c r="H88" s="82" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
@@ -5289,7 +5309,7 @@
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="236"/>
       <c r="B97" s="78" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="C97" s="79" t="s">
         <v>48</v>
@@ -5306,7 +5326,7 @@
       </c>
       <c r="G97" s="109"/>
       <c r="H97" s="110" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -5536,7 +5556,7 @@
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="236"/>
       <c r="B108" s="111" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C108" s="112"/>
       <c r="D108" s="113">
@@ -5551,7 +5571,7 @@
       </c>
       <c r="G108" s="112"/>
       <c r="H108" s="114" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -5702,7 +5722,7 @@
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="236"/>
       <c r="B116" s="184" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C116" s="185" t="s">
         <v>360</v>
@@ -5725,7 +5745,7 @@
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="236"/>
       <c r="B117" s="184" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C117" s="185" t="s">
         <v>360</v>
@@ -6022,115 +6042,112 @@
     <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="236"/>
       <c r="B133" s="106" t="s">
-        <v>526</v>
+        <v>600</v>
       </c>
       <c r="C133" s="107"/>
       <c r="D133" s="108">
         <v>2.95</v>
       </c>
       <c r="E133" s="107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F133" s="108">
         <f t="shared" ref="F133:F138" si="6">D133*E133</f>
-        <v>5.9</v>
+        <v>2.95</v>
       </c>
       <c r="G133" s="109"/>
-      <c r="H133" s="110" t="str">
-        <f>HYPERLINK("http://www.adafruit.com/products/899","http://www.adafruit.com/products/899")</f>
-        <v>http://www.adafruit.com/products/899</v>
+      <c r="H133" s="110" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="236"/>
       <c r="B134" s="106" t="s">
-        <v>127</v>
+        <v>606</v>
       </c>
       <c r="C134" s="107"/>
       <c r="D134" s="108">
-        <v>5.95</v>
+        <v>2.95</v>
       </c>
       <c r="E134" s="107">
         <v>1</v>
       </c>
       <c r="F134" s="108">
         <f t="shared" si="6"/>
-        <v>5.95</v>
+        <v>2.95</v>
       </c>
       <c r="G134" s="109"/>
       <c r="H134" s="110" t="s">
-        <v>128</v>
+        <v>607</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="236"/>
       <c r="B135" s="106" t="s">
-        <v>515</v>
+        <v>127</v>
       </c>
       <c r="C135" s="107"/>
       <c r="D135" s="108">
-        <v>4.95</v>
+        <v>5.95</v>
       </c>
       <c r="E135" s="107">
         <v>1</v>
       </c>
       <c r="F135" s="108">
         <f t="shared" si="6"/>
-        <v>4.95</v>
+        <v>5.95</v>
       </c>
       <c r="G135" s="109"/>
       <c r="H135" s="110" t="s">
-        <v>516</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="236"/>
       <c r="B136" s="106" t="s">
-        <v>466</v>
-      </c>
-      <c r="C136" s="107" t="s">
-        <v>468</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="C136" s="107"/>
       <c r="D136" s="108">
-        <v>34.950000000000003</v>
+        <v>4.95</v>
       </c>
       <c r="E136" s="107">
         <v>1</v>
       </c>
       <c r="F136" s="108">
         <f t="shared" si="6"/>
-        <v>34.950000000000003</v>
+        <v>4.95</v>
       </c>
       <c r="G136" s="109"/>
       <c r="H136" s="110" t="s">
-        <v>467</v>
+        <v>512</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="236"/>
       <c r="B137" s="106" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="C137" s="107"/>
       <c r="D137" s="108">
         <v>0.95</v>
       </c>
       <c r="E137" s="107">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F137" s="108">
         <f t="shared" si="6"/>
-        <v>0.95</v>
+        <v>1.9</v>
       </c>
       <c r="G137" s="109"/>
       <c r="H137" s="110" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="236"/>
       <c r="B138" s="106" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="C138" s="107"/>
       <c r="D138" s="108">
@@ -6145,7 +6162,7 @@
       </c>
       <c r="G138" s="109"/>
       <c r="H138" s="110" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -6199,7 +6216,7 @@
       </c>
       <c r="G141" s="109"/>
       <c r="H141" s="148" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
@@ -6667,7 +6684,7 @@
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="236"/>
       <c r="B164" s="78" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C164" s="79" t="s">
         <v>48</v>
@@ -6684,7 +6701,7 @@
       </c>
       <c r="G164" s="81"/>
       <c r="H164" s="82" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
@@ -6811,7 +6828,7 @@
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="237"/>
       <c r="B171" s="162" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C171" s="163"/>
       <c r="D171" s="199">
@@ -6821,153 +6838,151 @@
         <v>2</v>
       </c>
       <c r="F171" s="80">
-        <f t="shared" ref="F171:F172" si="8">D171*E171</f>
+        <f t="shared" ref="F171" si="8">D171*E171</f>
         <v>29.3</v>
       </c>
       <c r="G171" s="163"/>
       <c r="H171" s="149" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="237"/>
-      <c r="B172" s="184" t="s">
-        <v>602</v>
-      </c>
-      <c r="C172" s="185" t="s">
-        <v>601</v>
-      </c>
-      <c r="D172" s="223">
-        <v>33.25</v>
-      </c>
-      <c r="E172" s="224">
-        <v>0</v>
-      </c>
-      <c r="F172" s="186">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G172" s="185"/>
-      <c r="H172" s="225" t="s">
-        <v>487</v>
-      </c>
+      <c r="B172" s="161"/>
+      <c r="C172" s="159"/>
+      <c r="D172" s="216"/>
+      <c r="E172" s="160"/>
+      <c r="F172" s="80"/>
+      <c r="G172" s="159"/>
+      <c r="H172" s="217"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A173" s="237"/>
-      <c r="B173" s="161"/>
-      <c r="C173" s="159"/>
-      <c r="D173" s="216"/>
-      <c r="E173" s="160"/>
-      <c r="F173" s="80"/>
-      <c r="G173" s="159"/>
-      <c r="H173" s="217"/>
+      <c r="A173" s="236"/>
+      <c r="B173" s="78" t="s">
+        <v>569</v>
+      </c>
+      <c r="C173" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="D173" s="80">
+        <v>1.4</v>
+      </c>
+      <c r="E173" s="79">
+        <v>5</v>
+      </c>
+      <c r="F173" s="80">
+        <f>D173*E173</f>
+        <v>7</v>
+      </c>
+      <c r="G173" s="81"/>
+      <c r="H173" s="82" t="str">
+        <f>HYPERLINK("https://www.kjmagnetics.com/proddetail.asp?prod=D21B-N52","https://www.kjmagnetics.com/proddetail.asp?prod=D21B-N52")</f>
+        <v>https://www.kjmagnetics.com/proddetail.asp?prod=D21B-N52</v>
+      </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="236"/>
-      <c r="B174" s="78" t="s">
-        <v>574</v>
-      </c>
-      <c r="C174" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D174" s="80">
-        <v>1.4</v>
-      </c>
-      <c r="E174" s="79">
-        <v>5</v>
-      </c>
-      <c r="F174" s="80">
-        <f>D174*E174</f>
-        <v>7</v>
-      </c>
-      <c r="G174" s="81"/>
-      <c r="H174" s="82" t="str">
-        <f>HYPERLINK("https://www.kjmagnetics.com/proddetail.asp?prod=D21B-N52","https://www.kjmagnetics.com/proddetail.asp?prod=D21B-N52")</f>
-        <v>https://www.kjmagnetics.com/proddetail.asp?prod=D21B-N52</v>
-      </c>
+      <c r="B174" s="84"/>
+      <c r="C174" s="85"/>
+      <c r="D174" s="86"/>
+      <c r="E174" s="85"/>
+      <c r="F174" s="86"/>
+      <c r="G174" s="87"/>
+      <c r="H174" s="88"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="236"/>
-      <c r="B175" s="84"/>
-      <c r="C175" s="85"/>
-      <c r="D175" s="86"/>
-      <c r="E175" s="85"/>
-      <c r="F175" s="86"/>
-      <c r="G175" s="87"/>
-      <c r="H175" s="88"/>
+      <c r="B175" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="C175" s="79"/>
+      <c r="D175" s="80">
+        <v>23.39</v>
+      </c>
+      <c r="E175" s="83">
+        <v>1</v>
+      </c>
+      <c r="F175" s="80">
+        <f>D175*E175</f>
+        <v>23.39</v>
+      </c>
+      <c r="G175" s="81"/>
+      <c r="H175" s="96" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="236"/>
-      <c r="B176" s="78" t="s">
-        <v>157</v>
-      </c>
-      <c r="C176" s="79"/>
-      <c r="D176" s="80">
-        <v>23.39</v>
-      </c>
-      <c r="E176" s="83">
-        <v>1</v>
-      </c>
-      <c r="F176" s="80">
+      <c r="B176" s="106" t="s">
+        <v>159</v>
+      </c>
+      <c r="C176" s="107"/>
+      <c r="D176" s="108">
+        <v>19.53</v>
+      </c>
+      <c r="E176" s="134">
+        <v>1</v>
+      </c>
+      <c r="F176" s="108">
         <f>D176*E176</f>
-        <v>23.39</v>
-      </c>
-      <c r="G176" s="81"/>
-      <c r="H176" s="96" t="s">
-        <v>158</v>
+        <v>19.53</v>
+      </c>
+      <c r="G176" s="109"/>
+      <c r="H176" s="135" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A177" s="236"/>
       <c r="B177" s="106" t="s">
-        <v>159</v>
+        <v>522</v>
       </c>
       <c r="C177" s="107"/>
       <c r="D177" s="108">
-        <v>19.53</v>
-      </c>
-      <c r="E177" s="134">
-        <v>1</v>
+        <v>18.13</v>
+      </c>
+      <c r="E177" s="107">
+        <v>2</v>
       </c>
       <c r="F177" s="108">
         <f>D177*E177</f>
-        <v>19.53</v>
+        <v>36.26</v>
       </c>
       <c r="G177" s="109"/>
-      <c r="H177" s="135" t="s">
-        <v>160</v>
+      <c r="H177" s="110" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A178" s="236"/>
-      <c r="B178" s="106" t="s">
-        <v>527</v>
-      </c>
-      <c r="C178" s="107"/>
-      <c r="D178" s="108">
-        <v>18.13</v>
-      </c>
-      <c r="E178" s="107">
-        <v>2</v>
-      </c>
-      <c r="F178" s="108">
-        <f>D178*E178</f>
-        <v>36.26</v>
-      </c>
-      <c r="G178" s="109"/>
-      <c r="H178" s="110" t="s">
-        <v>161</v>
-      </c>
+      <c r="B178" s="123"/>
+      <c r="C178" s="123"/>
+      <c r="D178" s="124"/>
+      <c r="E178" s="136"/>
+      <c r="F178" s="108"/>
+      <c r="G178" s="125"/>
+      <c r="H178" s="137"/>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A179" s="236"/>
-      <c r="B179" s="123"/>
-      <c r="C179" s="123"/>
-      <c r="D179" s="124"/>
-      <c r="E179" s="136"/>
-      <c r="F179" s="124"/>
-      <c r="G179" s="125"/>
-      <c r="H179" s="137"/>
+      <c r="B179" s="84" t="s">
+        <v>466</v>
+      </c>
+      <c r="C179" s="85"/>
+      <c r="D179" s="86">
+        <v>149</v>
+      </c>
+      <c r="E179" s="95">
+        <v>1</v>
+      </c>
+      <c r="F179" s="108">
+        <f t="shared" ref="F179" si="9">D179*E179</f>
+        <v>149</v>
+      </c>
+      <c r="G179" s="87"/>
+      <c r="H179" s="225" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A180" s="236"/>
@@ -6976,9 +6991,9 @@
       <c r="D180" s="127"/>
       <c r="E180" s="126"/>
       <c r="F180" s="127"/>
-      <c r="G180" s="128">
-        <f>SUM(F128:F178)</f>
-        <v>6002.3000000000011</v>
+      <c r="G180" s="223">
+        <f>SUM(F128:F179)</f>
+        <v>6117.3000000000011</v>
       </c>
       <c r="H180" s="129"/>
     </row>
@@ -7007,10 +7022,10 @@
         <v>162</v>
       </c>
       <c r="B183" s="218" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C183" s="163" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D183" s="199">
         <v>108.99</v>
@@ -7019,7 +7034,7 @@
         <v>1</v>
       </c>
       <c r="F183" s="108">
-        <f t="shared" ref="F183:F194" si="9">D183*E183</f>
+        <f t="shared" ref="F183:F194" si="10">D183*E183</f>
         <v>108.99</v>
       </c>
       <c r="G183" s="163"/>
@@ -7049,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="F184" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>304.99</v>
       </c>
       <c r="G184" s="163"/>
@@ -7077,7 +7092,7 @@
         <v>1</v>
       </c>
       <c r="F185" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>157.99</v>
       </c>
       <c r="G185" s="163"/>
@@ -7105,7 +7120,7 @@
         <v>1</v>
       </c>
       <c r="F186" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>309.99</v>
       </c>
       <c r="G186" s="163"/>
@@ -7133,7 +7148,7 @@
         <v>1</v>
       </c>
       <c r="F187" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>448</v>
       </c>
       <c r="G187" s="163"/>
@@ -7194,7 +7209,7 @@
         <v>1</v>
       </c>
       <c r="F189" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.95</v>
       </c>
       <c r="G189" s="109"/>
@@ -7222,7 +7237,7 @@
         <v>1</v>
       </c>
       <c r="F190" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14.12</v>
       </c>
       <c r="G190" s="109"/>
@@ -7250,7 +7265,7 @@
         <v>1</v>
       </c>
       <c r="F191" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.99</v>
       </c>
       <c r="G191" s="109"/>
@@ -7278,7 +7293,7 @@
         <v>1</v>
       </c>
       <c r="F192" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>19.989999999999998</v>
       </c>
       <c r="G192" s="109"/>
@@ -7290,7 +7305,7 @@
     <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" s="236"/>
       <c r="B193" s="106" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="C193" s="107"/>
       <c r="D193" s="108">
@@ -7300,7 +7315,7 @@
         <v>1</v>
       </c>
       <c r="F193" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.29</v>
       </c>
       <c r="G193" s="109"/>
@@ -7321,7 +7336,7 @@
         <v>4</v>
       </c>
       <c r="F194" s="108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>23.96</v>
       </c>
       <c r="G194" s="134"/>
@@ -7368,16 +7383,16 @@
       </c>
       <c r="G196" s="144"/>
       <c r="H196" s="135" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" s="236"/>
       <c r="B197" s="56" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C197" s="143" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="D197" s="139">
         <v>329</v>
@@ -7471,7 +7486,7 @@
         <v>1</v>
       </c>
       <c r="F202" s="80">
-        <f t="shared" ref="F202:F244" si="10">D202*E202</f>
+        <f t="shared" ref="F202:F244" si="11">D202*E202</f>
         <v>19.93</v>
       </c>
       <c r="G202" s="81"/>
@@ -7513,7 +7528,7 @@
         <v>2</v>
       </c>
       <c r="F204" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.9</v>
       </c>
       <c r="G204" s="81"/>
@@ -7523,94 +7538,92 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" s="236"/>
-      <c r="B205" s="184" t="s">
-        <v>599</v>
-      </c>
-      <c r="C205" s="185" t="s">
-        <v>600</v>
-      </c>
-      <c r="D205" s="186">
-        <v>7.01</v>
-      </c>
-      <c r="E205" s="185">
-        <v>0</v>
-      </c>
-      <c r="F205" s="186">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G205" s="187"/>
-      <c r="H205" s="188" t="s">
-        <v>494</v>
+      <c r="B205" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="C205" s="79"/>
+      <c r="D205" s="80">
+        <v>0.32</v>
+      </c>
+      <c r="E205" s="79">
+        <v>10</v>
+      </c>
+      <c r="F205" s="80">
+        <f t="shared" si="11"/>
+        <v>3.2</v>
+      </c>
+      <c r="G205" s="81"/>
+      <c r="H205" s="82" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" s="236"/>
       <c r="B206" s="78" t="s">
-        <v>180</v>
+        <v>505</v>
       </c>
       <c r="C206" s="79"/>
       <c r="D206" s="80">
-        <v>0.32</v>
+        <v>0.04</v>
       </c>
       <c r="E206" s="79">
         <v>10</v>
       </c>
       <c r="F206" s="80">
-        <f t="shared" si="10"/>
-        <v>3.2</v>
+        <f t="shared" si="11"/>
+        <v>0.4</v>
       </c>
       <c r="G206" s="81"/>
       <c r="H206" s="82" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="236"/>
       <c r="B207" s="78" t="s">
-        <v>509</v>
+        <v>544</v>
       </c>
       <c r="C207" s="79"/>
       <c r="D207" s="80">
-        <v>0.04</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E207" s="79">
         <v>10</v>
       </c>
       <c r="F207" s="80">
-        <f t="shared" si="10"/>
-        <v>0.4</v>
+        <f t="shared" si="11"/>
+        <v>5.6999999999999993</v>
       </c>
       <c r="G207" s="81"/>
       <c r="H207" s="82" t="s">
-        <v>182</v>
+        <v>543</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="236"/>
       <c r="B208" s="78" t="s">
-        <v>549</v>
+        <v>595</v>
       </c>
       <c r="C208" s="79"/>
       <c r="D208" s="80">
-        <v>0.56999999999999995</v>
+        <v>0.04</v>
       </c>
       <c r="E208" s="79">
         <v>10</v>
       </c>
       <c r="F208" s="80">
-        <f t="shared" si="10"/>
-        <v>5.6999999999999993</v>
+        <f t="shared" si="11"/>
+        <v>0.4</v>
       </c>
       <c r="G208" s="81"/>
       <c r="H208" s="82" t="s">
-        <v>548</v>
+        <v>594</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="236"/>
       <c r="B209" s="78" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="C209" s="79"/>
       <c r="D209" s="80">
@@ -7620,138 +7633,138 @@
         <v>10</v>
       </c>
       <c r="F209" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.4</v>
       </c>
       <c r="G209" s="81"/>
       <c r="H209" s="82" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" s="236"/>
       <c r="B210" s="78" t="s">
-        <v>605</v>
+        <v>504</v>
       </c>
       <c r="C210" s="79"/>
       <c r="D210" s="80">
-        <v>0.04</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="E210" s="79">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F210" s="80">
-        <f t="shared" si="10"/>
-        <v>0.4</v>
+        <f t="shared" si="11"/>
+        <v>0.72</v>
       </c>
       <c r="G210" s="81"/>
       <c r="H210" s="82" t="s">
-        <v>606</v>
+        <v>506</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" s="236"/>
       <c r="B211" s="78" t="s">
-        <v>508</v>
+        <v>183</v>
       </c>
       <c r="C211" s="79"/>
       <c r="D211" s="80">
-        <v>2.8799999999999999E-2</v>
+        <v>1.67</v>
       </c>
       <c r="E211" s="79">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F211" s="80">
-        <f t="shared" si="10"/>
-        <v>0.72</v>
+        <f t="shared" si="11"/>
+        <v>16.7</v>
       </c>
       <c r="G211" s="81"/>
       <c r="H211" s="82" t="s">
-        <v>510</v>
+        <v>184</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" s="236"/>
       <c r="B212" s="78" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C212" s="79"/>
       <c r="D212" s="80">
-        <v>1.67</v>
+        <v>37.4</v>
       </c>
       <c r="E212" s="79">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F212" s="80">
-        <f t="shared" si="10"/>
-        <v>16.7</v>
+        <f t="shared" si="11"/>
+        <v>37.4</v>
       </c>
       <c r="G212" s="81"/>
       <c r="H212" s="82" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213" s="236"/>
       <c r="B213" s="78" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C213" s="79"/>
       <c r="D213" s="80">
-        <v>37.4</v>
-      </c>
-      <c r="E213" s="79">
+        <v>14.95</v>
+      </c>
+      <c r="E213" s="83">
         <v>1</v>
       </c>
       <c r="F213" s="80">
-        <f t="shared" si="10"/>
-        <v>37.4</v>
+        <f t="shared" si="11"/>
+        <v>14.95</v>
       </c>
       <c r="G213" s="81"/>
       <c r="H213" s="82" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" s="236"/>
       <c r="B214" s="78" t="s">
-        <v>187</v>
+        <v>568</v>
       </c>
       <c r="C214" s="79"/>
       <c r="D214" s="80">
-        <v>14.95</v>
+        <v>16.54</v>
       </c>
       <c r="E214" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F214" s="80">
-        <f t="shared" si="10"/>
-        <v>14.95</v>
+        <f t="shared" si="11"/>
+        <v>33.08</v>
       </c>
       <c r="G214" s="81"/>
       <c r="H214" s="82" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" s="236"/>
       <c r="B215" s="78" t="s">
-        <v>573</v>
+        <v>604</v>
       </c>
       <c r="C215" s="79"/>
       <c r="D215" s="80">
-        <v>16.54</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="E215" s="83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F215" s="80">
-        <f t="shared" si="10"/>
-        <v>33.08</v>
+        <f t="shared" si="11"/>
+        <v>73.099999999999994</v>
       </c>
       <c r="G215" s="81"/>
       <c r="H215" s="82" t="s">
-        <v>189</v>
+        <v>605</v>
       </c>
     </row>
     <row r="216" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7767,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="F216" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>33.35</v>
       </c>
       <c r="G216" s="81"/>
@@ -7788,7 +7801,7 @@
         <v>2</v>
       </c>
       <c r="F217" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.194</v>
       </c>
       <c r="G217" s="109"/>
@@ -7810,7 +7823,7 @@
         <v>2</v>
       </c>
       <c r="F218" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16.62</v>
       </c>
       <c r="G218" s="109"/>
@@ -7831,7 +7844,7 @@
         <v>2</v>
       </c>
       <c r="F219" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.52</v>
       </c>
       <c r="G219" s="109"/>
@@ -7852,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="F220" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
       <c r="G220" s="109"/>
@@ -7873,7 +7886,7 @@
         <v>2</v>
       </c>
       <c r="F221" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>49.28</v>
       </c>
       <c r="G221" s="109"/>
@@ -7894,7 +7907,7 @@
         <v>1</v>
       </c>
       <c r="F222" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.81</v>
       </c>
       <c r="G222" s="109"/>
@@ -7905,7 +7918,7 @@
     <row r="223" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A223" s="236"/>
       <c r="B223" s="106" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="C223" s="107"/>
       <c r="D223" s="108">
@@ -7915,7 +7928,7 @@
         <v>2</v>
       </c>
       <c r="F223" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>78</v>
       </c>
       <c r="G223" s="109"/>
@@ -7936,7 +7949,7 @@
         <v>2</v>
       </c>
       <c r="F224" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>49.98</v>
       </c>
       <c r="G224" s="109"/>
@@ -7947,7 +7960,7 @@
     <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" s="236"/>
       <c r="B225" s="106" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="C225" s="107"/>
       <c r="D225" s="108">
@@ -7957,7 +7970,7 @@
         <v>1</v>
       </c>
       <c r="F225" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>20</v>
       </c>
       <c r="G225" s="109"/>
@@ -7978,7 +7991,7 @@
         <v>1</v>
       </c>
       <c r="F226" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="G226" s="109"/>
@@ -7989,7 +8002,7 @@
     <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" s="236"/>
       <c r="B227" s="106" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="C227" s="107"/>
       <c r="D227" s="108">
@@ -7999,7 +8012,7 @@
         <v>1</v>
       </c>
       <c r="F227" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="G227" s="109"/>
@@ -8020,7 +8033,7 @@
         <v>1</v>
       </c>
       <c r="F228" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.23</v>
       </c>
       <c r="G228" s="109"/>
@@ -8041,7 +8054,7 @@
         <v>1</v>
       </c>
       <c r="F229" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11.53</v>
       </c>
       <c r="G229" s="109"/>
@@ -8062,7 +8075,7 @@
         <v>1</v>
       </c>
       <c r="F230" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.26</v>
       </c>
       <c r="G230" s="109"/>
@@ -8073,7 +8086,7 @@
     <row r="231" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A231" s="236"/>
       <c r="B231" s="106" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="C231" s="107"/>
       <c r="D231" s="108">
@@ -8083,7 +8096,7 @@
         <v>2</v>
       </c>
       <c r="F231" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>33.880000000000003</v>
       </c>
       <c r="G231" s="109"/>
@@ -8104,7 +8117,7 @@
         <v>5</v>
       </c>
       <c r="F232" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.45</v>
       </c>
       <c r="G232" s="109"/>
@@ -8125,7 +8138,7 @@
         <v>25</v>
       </c>
       <c r="F233" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.8449999999999998</v>
       </c>
       <c r="G233" s="109"/>
@@ -8146,7 +8159,7 @@
         <v>5</v>
       </c>
       <c r="F234" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.9</v>
       </c>
       <c r="G234" s="109"/>
@@ -8167,12 +8180,12 @@
         <v>5</v>
       </c>
       <c r="F235" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.9499999999999997</v>
       </c>
       <c r="G235" s="109"/>
       <c r="H235" s="110" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.35">
@@ -8188,7 +8201,7 @@
         <v>10</v>
       </c>
       <c r="F236" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.52</v>
       </c>
       <c r="G236" s="109"/>
@@ -8202,7 +8215,7 @@
         <v>399</v>
       </c>
       <c r="C237" s="107" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D237" s="108">
         <v>20.170000000000002</v>
@@ -8211,7 +8224,7 @@
         <v>1</v>
       </c>
       <c r="F237" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>20.170000000000002</v>
       </c>
       <c r="G237" s="109"/>
@@ -8225,7 +8238,7 @@
         <v>401</v>
       </c>
       <c r="C238" s="107" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D238" s="108">
         <v>20.350000000000001</v>
@@ -8234,7 +8247,7 @@
         <v>1</v>
       </c>
       <c r="F238" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>20.350000000000001</v>
       </c>
       <c r="G238" s="109"/>
@@ -8248,7 +8261,7 @@
         <v>403</v>
       </c>
       <c r="C239" s="107" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D239" s="99">
         <v>20.18</v>
@@ -8257,7 +8270,7 @@
         <v>1</v>
       </c>
       <c r="F239" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>20.18</v>
       </c>
       <c r="G239" s="100"/>
@@ -8271,7 +8284,7 @@
         <v>405</v>
       </c>
       <c r="C240" s="107" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D240" s="99">
         <v>12.03</v>
@@ -8280,7 +8293,7 @@
         <v>1</v>
       </c>
       <c r="F240" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.03</v>
       </c>
       <c r="G240" s="100"/>
@@ -8291,10 +8304,10 @@
     <row r="241" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A241" s="236"/>
       <c r="B241" s="97" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="C241" s="107" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D241" s="99">
         <v>18.75</v>
@@ -8303,7 +8316,7 @@
         <v>1</v>
       </c>
       <c r="F241" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>18.75</v>
       </c>
       <c r="G241" s="100"/>
@@ -8317,7 +8330,7 @@
         <v>407</v>
       </c>
       <c r="C242" s="107" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D242" s="99">
         <v>0.82</v>
@@ -8326,7 +8339,7 @@
         <v>2</v>
       </c>
       <c r="F242" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.64</v>
       </c>
       <c r="G242" s="100"/>
@@ -8337,10 +8350,10 @@
     <row r="243" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A243" s="236"/>
       <c r="B243" s="97" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="C243" s="185" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="D243" s="99">
         <v>13.1</v>
@@ -8349,18 +8362,18 @@
         <v>1</v>
       </c>
       <c r="F243" s="108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.1</v>
       </c>
       <c r="G243" s="100"/>
       <c r="H243" s="101" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A244" s="236"/>
       <c r="B244" s="97" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="C244" s="185" t="s">
         <v>225</v>
@@ -8372,7 +8385,7 @@
         <v>1</v>
       </c>
       <c r="F244" s="99">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>276.41000000000003</v>
       </c>
       <c r="G244" s="100"/>
@@ -8403,7 +8416,7 @@
         <v>1</v>
       </c>
       <c r="F246" s="108">
-        <f t="shared" ref="F246:F253" si="11">D246*E246</f>
+        <f t="shared" ref="F246:F253" si="12">D246*E246</f>
         <v>18.399999999999999</v>
       </c>
       <c r="G246" s="109"/>
@@ -8424,7 +8437,7 @@
         <v>1</v>
       </c>
       <c r="F247" s="108">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.96</v>
       </c>
       <c r="G247" s="109"/>
@@ -8435,7 +8448,7 @@
     <row r="248" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A248" s="236"/>
       <c r="B248" s="106" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="C248" s="107"/>
       <c r="D248" s="108">
@@ -8445,7 +8458,7 @@
         <v>1</v>
       </c>
       <c r="F248" s="108">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>18.48</v>
       </c>
       <c r="G248" s="109"/>
@@ -8456,7 +8469,7 @@
     <row r="249" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A249" s="236"/>
       <c r="B249" s="106" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="C249" s="107"/>
       <c r="D249" s="108">
@@ -8466,7 +8479,7 @@
         <v>1</v>
       </c>
       <c r="F249" s="108">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.86</v>
       </c>
       <c r="G249" s="109"/>
@@ -8487,7 +8500,7 @@
         <v>3</v>
       </c>
       <c r="F250" s="99">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24.630000000000003</v>
       </c>
       <c r="G250" s="100"/>
@@ -8508,7 +8521,7 @@
         <v>1</v>
       </c>
       <c r="F251" s="118">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>28.26</v>
       </c>
       <c r="G251" s="119"/>
@@ -8529,7 +8542,7 @@
         <v>1</v>
       </c>
       <c r="F252" s="118">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.69</v>
       </c>
       <c r="G252" s="119"/>
@@ -8540,7 +8553,7 @@
     <row r="253" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A253" s="236"/>
       <c r="B253" s="116" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C253" s="117"/>
       <c r="D253" s="118">
@@ -8550,12 +8563,12 @@
         <v>2</v>
       </c>
       <c r="F253" s="118">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.98</v>
       </c>
       <c r="G253" s="119"/>
       <c r="H253" s="142" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.35">
@@ -8570,45 +8583,45 @@
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A255" s="236"/>
-      <c r="B255" s="106" t="s">
-        <v>567</v>
-      </c>
-      <c r="C255" s="107"/>
-      <c r="D255" s="108">
-        <v>1.08</v>
-      </c>
-      <c r="E255" s="107">
-        <v>2</v>
+      <c r="B255" s="84" t="s">
+        <v>608</v>
+      </c>
+      <c r="C255" s="85"/>
+      <c r="D255" s="86">
+        <v>0.93</v>
+      </c>
+      <c r="E255" s="85">
+        <v>1</v>
       </c>
       <c r="F255" s="108">
-        <f t="shared" ref="F255:F260" si="12">D255*E255</f>
-        <v>2.16</v>
-      </c>
-      <c r="G255" s="109"/>
-      <c r="H255" s="135" t="str">
-        <f>HYPERLINK("http://www.monoprice.com/Product?c_id=103&amp;cp_id=10303&amp;cs_id=1030302&amp;p_id=5446&amp;seq=1&amp;format=2","http://www.monoprice.com/Product?c_id=103&amp;cp_id=10303&amp;cs_id=1030302&amp;p_id=5446&amp;seq=1&amp;format=2")</f>
-        <v>http://www.monoprice.com/Product?c_id=103&amp;cp_id=10303&amp;cs_id=1030302&amp;p_id=5446&amp;seq=1&amp;format=2</v>
+        <f t="shared" ref="F255:F261" si="13">D255*E255</f>
+        <v>0.93</v>
+      </c>
+      <c r="G255" s="87"/>
+      <c r="H255" s="88" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A256" s="236"/>
       <c r="B256" s="106" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C256" s="107"/>
       <c r="D256" s="108">
-        <v>0.74</v>
+        <v>1.08</v>
       </c>
       <c r="E256" s="107">
         <v>2</v>
       </c>
       <c r="F256" s="108">
-        <f t="shared" si="12"/>
-        <v>1.48</v>
+        <f t="shared" si="13"/>
+        <v>2.16</v>
       </c>
       <c r="G256" s="109"/>
-      <c r="H256" s="135" t="s">
-        <v>234</v>
+      <c r="H256" s="135" t="str">
+        <f>HYPERLINK("http://www.monoprice.com/Product?c_id=103&amp;cp_id=10303&amp;cs_id=1030302&amp;p_id=5446&amp;seq=1&amp;format=2","http://www.monoprice.com/Product?c_id=103&amp;cp_id=10303&amp;cs_id=1030302&amp;p_id=5446&amp;seq=1&amp;format=2")</f>
+        <v>http://www.monoprice.com/Product?c_id=103&amp;cp_id=10303&amp;cs_id=1030302&amp;p_id=5446&amp;seq=1&amp;format=2</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.35">
@@ -8618,147 +8631,158 @@
       </c>
       <c r="C257" s="107"/>
       <c r="D257" s="108">
-        <v>0.69</v>
-      </c>
-      <c r="E257" s="134">
-        <v>1</v>
+        <v>0.74</v>
+      </c>
+      <c r="E257" s="107">
+        <v>2</v>
       </c>
       <c r="F257" s="108">
-        <f>D257*E257</f>
-        <v>0.69</v>
+        <f t="shared" si="13"/>
+        <v>1.48</v>
       </c>
       <c r="G257" s="109"/>
       <c r="H257" s="135" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A258" s="236"/>
       <c r="B258" s="106" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="C258" s="107"/>
       <c r="D258" s="108">
-        <v>0.79</v>
+        <v>0.69</v>
       </c>
       <c r="E258" s="134">
         <v>1</v>
       </c>
       <c r="F258" s="108">
         <f>D258*E258</f>
-        <v>0.79</v>
+        <v>0.69</v>
       </c>
       <c r="G258" s="109"/>
       <c r="H258" s="135" t="s">
-        <v>536</v>
+        <v>236</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A259" s="236"/>
       <c r="B259" s="106" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C259" s="107"/>
       <c r="D259" s="108">
-        <v>1.95</v>
+        <v>0.79</v>
       </c>
       <c r="E259" s="134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F259" s="108">
         <f>D259*E259</f>
-        <v>3.9</v>
+        <v>0.79</v>
       </c>
       <c r="G259" s="109"/>
       <c r="H259" s="135" t="s">
-        <v>460</v>
+        <v>531</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A260" s="236"/>
       <c r="B260" s="106" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C260" s="107"/>
       <c r="D260" s="108">
-        <v>5.78</v>
-      </c>
-      <c r="E260" s="107">
-        <v>1</v>
+        <v>1.95</v>
+      </c>
+      <c r="E260" s="134">
+        <v>2</v>
       </c>
       <c r="F260" s="108">
-        <f t="shared" si="12"/>
-        <v>5.78</v>
+        <f>D260*E260</f>
+        <v>3.9</v>
       </c>
       <c r="G260" s="109"/>
       <c r="H260" s="135" t="s">
-        <v>235</v>
+        <v>460</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A261" s="236"/>
       <c r="B261" s="106" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C261" s="107"/>
       <c r="D261" s="108">
+        <v>5.78</v>
+      </c>
+      <c r="E261" s="107">
+        <v>1</v>
+      </c>
+      <c r="F261" s="108">
+        <f t="shared" si="13"/>
+        <v>5.78</v>
+      </c>
+      <c r="G261" s="109"/>
+      <c r="H261" s="135" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A262" s="236"/>
+      <c r="B262" s="106" t="s">
+        <v>560</v>
+      </c>
+      <c r="C262" s="107"/>
+      <c r="D262" s="108">
         <v>1.7</v>
       </c>
-      <c r="E261" s="107">
+      <c r="E262" s="107">
         <v>2</v>
       </c>
-      <c r="F261" s="108">
-        <f>D261*E261</f>
+      <c r="F262" s="108">
+        <f>D262*E262</f>
         <v>3.4</v>
       </c>
-      <c r="G261" s="109"/>
-      <c r="H261" s="135" t="str">
+      <c r="G262" s="109"/>
+      <c r="H262" s="135" t="str">
         <f>HYPERLINK("http://www.monoprice.com/product?c_id=102&amp;cp_id=10208&amp;cs_id=1020807&amp;p_id=11239&amp;seq=1&amp;format=2","http://www.monoprice.com/product?c_id=102&amp;cp_id=10208&amp;cs_id=1020807&amp;p_id=11239&amp;seq=1&amp;format=2")</f>
         <v>http://www.monoprice.com/product?c_id=102&amp;cp_id=10208&amp;cs_id=1020807&amp;p_id=11239&amp;seq=1&amp;format=2</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A262" s="236"/>
-      <c r="B262" s="106"/>
-      <c r="C262" s="107"/>
-      <c r="D262" s="108"/>
-      <c r="E262" s="134"/>
-      <c r="F262" s="108"/>
-      <c r="G262" s="109"/>
-      <c r="H262" s="135"/>
-    </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A263" s="47"/>
-      <c r="B263" s="33"/>
-      <c r="C263" s="33"/>
-      <c r="D263" s="35"/>
-      <c r="E263" s="41"/>
-      <c r="F263" s="35"/>
-      <c r="G263" s="35"/>
-      <c r="H263" s="48"/>
+      <c r="A263" s="236"/>
+      <c r="B263" s="106"/>
+      <c r="C263" s="107"/>
+      <c r="D263" s="108"/>
+      <c r="E263" s="134"/>
+      <c r="F263" s="108"/>
+      <c r="G263" s="109"/>
+      <c r="H263" s="135"/>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A264" s="49"/>
-      <c r="B264" s="36"/>
-      <c r="C264" s="36"/>
-      <c r="D264" s="50"/>
-      <c r="E264" s="36"/>
-      <c r="F264" s="50"/>
-      <c r="G264" s="37">
-        <f>SUM(F183:F263)</f>
-        <v>3019.7790000000009</v>
-      </c>
-      <c r="H264" s="38"/>
+      <c r="A264" s="47"/>
+      <c r="B264" s="33"/>
+      <c r="C264" s="33"/>
+      <c r="D264" s="35"/>
+      <c r="E264" s="41"/>
+      <c r="F264" s="35"/>
+      <c r="G264" s="35"/>
+      <c r="H264" s="48"/>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A265" s="39"/>
-      <c r="B265" s="39"/>
-      <c r="C265" s="39"/>
-      <c r="D265" s="40"/>
-      <c r="E265" s="39"/>
-      <c r="F265" s="40"/>
-      <c r="G265" s="40"/>
-      <c r="H265" s="39"/>
+      <c r="A265" s="49"/>
+      <c r="B265" s="36"/>
+      <c r="C265" s="36"/>
+      <c r="D265" s="50"/>
+      <c r="E265" s="36"/>
+      <c r="F265" s="50"/>
+      <c r="G265" s="37">
+        <f>SUM(F183:F264)</f>
+        <v>3093.8090000000007</v>
+      </c>
+      <c r="H265" s="38"/>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A266" s="39"/>
@@ -8770,40 +8794,40 @@
       <c r="G266" s="40"/>
       <c r="H266" s="39"/>
     </row>
-    <row r="267" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A267" s="242" t="s">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A267" s="39"/>
+      <c r="B267" s="39"/>
+      <c r="C267" s="39"/>
+      <c r="D267" s="40"/>
+      <c r="E267" s="39"/>
+      <c r="F267" s="40"/>
+      <c r="G267" s="40"/>
+      <c r="H267" s="39"/>
+    </row>
+    <row r="268" spans="1:8" ht="26" x14ac:dyDescent="0.6">
+      <c r="A268" s="242" t="s">
         <v>237</v>
       </c>
-      <c r="B267" s="243"/>
-      <c r="C267" s="201"/>
-      <c r="D267" s="202"/>
-      <c r="E267" s="201"/>
-      <c r="F267" s="252">
-        <f>SUM(G19:G264)</f>
-        <v>14446.218999999997</v>
-      </c>
-      <c r="G267" s="253"/>
-      <c r="H267" s="39"/>
-    </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A268" s="39"/>
-      <c r="B268" s="39"/>
-      <c r="C268" s="39"/>
-      <c r="D268" s="39"/>
-      <c r="E268" s="39"/>
-      <c r="F268" s="39"/>
-      <c r="G268" s="39"/>
+      <c r="B268" s="243"/>
+      <c r="C268" s="201"/>
+      <c r="D268" s="202"/>
+      <c r="E268" s="201"/>
+      <c r="F268" s="252">
+        <f>SUM(G19:G265)</f>
+        <v>14635.248999999998</v>
+      </c>
+      <c r="G268" s="253"/>
       <c r="H268" s="39"/>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A269" s="39"/>
       <c r="B269" s="39"/>
       <c r="C269" s="39"/>
-      <c r="D269" s="40"/>
+      <c r="D269" s="39"/>
       <c r="E269" s="39"/>
-      <c r="F269" s="40"/>
-      <c r="G269" s="40"/>
-      <c r="H269" s="51"/>
+      <c r="F269" s="39"/>
+      <c r="G269" s="39"/>
+      <c r="H269" s="39"/>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A270" s="39"/>
@@ -8813,7 +8837,7 @@
       <c r="E270" s="39"/>
       <c r="F270" s="40"/>
       <c r="G270" s="40"/>
-      <c r="H270" s="39"/>
+      <c r="H270" s="51"/>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A271" s="39"/>
@@ -8825,514 +8849,503 @@
       <c r="G271" s="40"/>
       <c r="H271" s="39"/>
     </row>
-    <row r="272" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A272" s="244"/>
-      <c r="B272" s="245"/>
-      <c r="C272" s="245"/>
-      <c r="D272" s="245"/>
-      <c r="E272" s="245"/>
-      <c r="F272" s="245"/>
-      <c r="G272" s="245"/>
-      <c r="H272" s="246"/>
-    </row>
-    <row r="273" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A273" s="247" t="s">
-        <v>488</v>
-      </c>
-      <c r="B273" s="248"/>
-      <c r="C273" s="248"/>
-      <c r="D273" s="248"/>
-      <c r="E273" s="248"/>
-      <c r="F273" s="248"/>
-      <c r="G273" s="248"/>
-      <c r="H273" s="249"/>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A272" s="39"/>
+      <c r="B272" s="39"/>
+      <c r="C272" s="39"/>
+      <c r="D272" s="40"/>
+      <c r="E272" s="39"/>
+      <c r="F272" s="40"/>
+      <c r="G272" s="40"/>
+      <c r="H272" s="39"/>
+    </row>
+    <row r="273" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A273" s="244"/>
+      <c r="B273" s="245"/>
+      <c r="C273" s="245"/>
+      <c r="D273" s="245"/>
+      <c r="E273" s="245"/>
+      <c r="F273" s="245"/>
+      <c r="G273" s="245"/>
+      <c r="H273" s="246"/>
     </row>
     <row r="274" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A274" s="254" t="s">
-        <v>528</v>
-      </c>
-      <c r="B274" s="255"/>
-      <c r="C274" s="255"/>
-      <c r="D274" s="255"/>
-      <c r="E274" s="255"/>
-      <c r="F274" s="255"/>
-      <c r="G274" s="255"/>
-      <c r="H274" s="256"/>
-    </row>
-    <row r="275" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A275" s="49"/>
-      <c r="B275" s="36"/>
-      <c r="C275" s="36"/>
-      <c r="D275" s="203" t="s">
+      <c r="A274" s="247" t="s">
+        <v>485</v>
+      </c>
+      <c r="B274" s="248"/>
+      <c r="C274" s="248"/>
+      <c r="D274" s="248"/>
+      <c r="E274" s="248"/>
+      <c r="F274" s="248"/>
+      <c r="G274" s="248"/>
+      <c r="H274" s="249"/>
+    </row>
+    <row r="275" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A275" s="254" t="s">
+        <v>523</v>
+      </c>
+      <c r="B275" s="255"/>
+      <c r="C275" s="255"/>
+      <c r="D275" s="255"/>
+      <c r="E275" s="255"/>
+      <c r="F275" s="255"/>
+      <c r="G275" s="255"/>
+      <c r="H275" s="256"/>
+    </row>
+    <row r="276" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A276" s="49"/>
+      <c r="B276" s="36"/>
+      <c r="C276" s="36"/>
+      <c r="D276" s="203" t="s">
         <v>4</v>
       </c>
-      <c r="E275" s="204" t="s">
+      <c r="E276" s="204" t="s">
         <v>5</v>
       </c>
-      <c r="F275" s="203" t="s">
+      <c r="F276" s="203" t="s">
         <v>6</v>
       </c>
-      <c r="G275" s="203" t="s">
+      <c r="G276" s="203" t="s">
         <v>7</v>
       </c>
-      <c r="H275" s="205" t="s">
+      <c r="H276" s="205" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A276" s="250" t="s">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A277" s="250" t="s">
+        <v>467</v>
+      </c>
+      <c r="B277" s="184" t="s">
+        <v>238</v>
+      </c>
+      <c r="C277" s="185" t="s">
+        <v>470</v>
+      </c>
+      <c r="D277" s="186">
+        <v>1068</v>
+      </c>
+      <c r="E277" s="185">
+        <v>1</v>
+      </c>
+      <c r="F277" s="186">
+        <f>D277*E277</f>
+        <v>1068</v>
+      </c>
+      <c r="G277" s="187"/>
+      <c r="H277" s="152" t="s">
         <v>469</v>
       </c>
-      <c r="B276" s="184" t="s">
-        <v>238</v>
-      </c>
-      <c r="C276" s="185" t="s">
-        <v>472</v>
-      </c>
-      <c r="D276" s="186">
-        <v>1068</v>
-      </c>
-      <c r="E276" s="185">
-        <v>1</v>
-      </c>
-      <c r="F276" s="186">
-        <f>D276*E276</f>
-        <v>1068</v>
-      </c>
-      <c r="G276" s="187"/>
-      <c r="H276" s="152" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="277" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A277" s="250"/>
-      <c r="B277" s="28"/>
-      <c r="C277" s="29"/>
-      <c r="D277" s="52"/>
-      <c r="E277" s="53"/>
-      <c r="F277" s="52"/>
-      <c r="G277" s="54"/>
-      <c r="H277" s="55"/>
     </row>
     <row r="278" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A278" s="250"/>
-      <c r="B278" s="28" t="s">
-        <v>240</v>
-      </c>
+      <c r="B278" s="28"/>
       <c r="C278" s="29"/>
-      <c r="D278" s="52">
-        <v>528.99</v>
-      </c>
-      <c r="E278" s="53">
-        <v>1</v>
-      </c>
-      <c r="F278" s="52">
-        <f>D278*E278</f>
-        <v>528.99</v>
-      </c>
+      <c r="D278" s="52"/>
+      <c r="E278" s="53"/>
+      <c r="F278" s="52"/>
       <c r="G278" s="54"/>
-      <c r="H278" s="55" t="s">
-        <v>241</v>
-      </c>
+      <c r="H278" s="55"/>
     </row>
     <row r="279" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A279" s="250"/>
-      <c r="B279" s="28"/>
+      <c r="B279" s="28" t="s">
+        <v>240</v>
+      </c>
       <c r="C279" s="29"/>
-      <c r="D279" s="52"/>
-      <c r="E279" s="53"/>
-      <c r="F279" s="52"/>
+      <c r="D279" s="52">
+        <v>528.99</v>
+      </c>
+      <c r="E279" s="53">
+        <v>1</v>
+      </c>
+      <c r="F279" s="52">
+        <f>D279*E279</f>
+        <v>528.99</v>
+      </c>
       <c r="G279" s="54"/>
-      <c r="H279" s="55"/>
+      <c r="H279" s="55" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="280" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A280" s="250"/>
-      <c r="B280" s="28" t="s">
-        <v>555</v>
-      </c>
+      <c r="B280" s="28"/>
       <c r="C280" s="29"/>
-      <c r="D280" s="52">
-        <v>49.99</v>
-      </c>
-      <c r="E280" s="53">
-        <v>1</v>
-      </c>
-      <c r="F280" s="52">
-        <f t="shared" ref="F280:F294" si="13">D280*E280</f>
-        <v>49.99</v>
-      </c>
+      <c r="D280" s="52"/>
+      <c r="E280" s="53"/>
+      <c r="F280" s="52"/>
       <c r="G280" s="54"/>
-      <c r="H280" s="55" t="s">
-        <v>242</v>
-      </c>
+      <c r="H280" s="55"/>
     </row>
     <row r="281" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A281" s="250"/>
-      <c r="B281" s="191" t="s">
-        <v>578</v>
-      </c>
-      <c r="C281" s="192"/>
-      <c r="D281" s="193">
-        <v>1.59</v>
-      </c>
-      <c r="E281" s="194">
-        <v>1</v>
-      </c>
-      <c r="F281" s="193">
-        <f t="shared" si="13"/>
-        <v>1.59</v>
-      </c>
-      <c r="G281" s="195"/>
-      <c r="H281" s="196" t="s">
-        <v>579</v>
+      <c r="B281" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="C281" s="29"/>
+      <c r="D281" s="52">
+        <v>49.99</v>
+      </c>
+      <c r="E281" s="53">
+        <v>1</v>
+      </c>
+      <c r="F281" s="52">
+        <f t="shared" ref="F281:F295" si="14">D281*E281</f>
+        <v>49.99</v>
+      </c>
+      <c r="G281" s="54"/>
+      <c r="H281" s="55" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="282" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A282" s="250"/>
-      <c r="B282" s="28"/>
-      <c r="C282" s="29"/>
-      <c r="D282" s="52"/>
-      <c r="E282" s="53"/>
-      <c r="F282" s="52"/>
-      <c r="G282" s="54"/>
-      <c r="H282" s="55"/>
+      <c r="B282" s="191" t="s">
+        <v>573</v>
+      </c>
+      <c r="C282" s="192"/>
+      <c r="D282" s="193">
+        <v>1.59</v>
+      </c>
+      <c r="E282" s="194">
+        <v>1</v>
+      </c>
+      <c r="F282" s="193">
+        <f t="shared" si="14"/>
+        <v>1.59</v>
+      </c>
+      <c r="G282" s="195"/>
+      <c r="H282" s="196" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="283" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A283" s="250"/>
-      <c r="B283" s="28" t="s">
-        <v>243</v>
-      </c>
+      <c r="B283" s="28"/>
       <c r="C283" s="29"/>
-      <c r="D283" s="52">
-        <v>32.49</v>
-      </c>
-      <c r="E283" s="53">
-        <v>1</v>
-      </c>
-      <c r="F283" s="52">
-        <f t="shared" si="13"/>
-        <v>32.49</v>
-      </c>
+      <c r="D283" s="52"/>
+      <c r="E283" s="53"/>
+      <c r="F283" s="52"/>
       <c r="G283" s="54"/>
-      <c r="H283" s="152" t="s">
-        <v>453</v>
-      </c>
+      <c r="H283" s="55"/>
     </row>
     <row r="284" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A284" s="250"/>
       <c r="B284" s="28" t="s">
-        <v>451</v>
+        <v>243</v>
       </c>
       <c r="C284" s="29"/>
       <c r="D284" s="52">
-        <v>9.9700000000000006</v>
+        <v>32.49</v>
       </c>
       <c r="E284" s="53">
         <v>1</v>
       </c>
       <c r="F284" s="52">
-        <f t="shared" si="13"/>
-        <v>9.9700000000000006</v>
+        <f t="shared" si="14"/>
+        <v>32.49</v>
       </c>
       <c r="G284" s="54"/>
-      <c r="H284" s="55" t="s">
-        <v>452</v>
+      <c r="H284" s="152" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="285" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A285" s="250"/>
-      <c r="B285" s="191" t="s">
-        <v>580</v>
-      </c>
-      <c r="C285" s="192"/>
-      <c r="D285" s="193">
-        <v>16.989999999999998</v>
-      </c>
-      <c r="E285" s="194">
-        <v>1</v>
-      </c>
-      <c r="F285" s="193">
-        <f t="shared" si="13"/>
-        <v>16.989999999999998</v>
-      </c>
-      <c r="G285" s="195"/>
-      <c r="H285" s="196" t="s">
-        <v>581</v>
+      <c r="B285" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="C285" s="29"/>
+      <c r="D285" s="52">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="E285" s="53">
+        <v>1</v>
+      </c>
+      <c r="F285" s="52">
+        <f t="shared" si="14"/>
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="G285" s="54"/>
+      <c r="H285" s="55" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="286" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A286" s="250"/>
-      <c r="B286" s="28"/>
-      <c r="C286" s="29"/>
-      <c r="D286" s="52"/>
-      <c r="E286" s="53"/>
-      <c r="F286" s="52"/>
-      <c r="G286" s="54"/>
-      <c r="H286" s="55"/>
-    </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B286" s="191" t="s">
+        <v>575</v>
+      </c>
+      <c r="C286" s="192"/>
+      <c r="D286" s="193">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E286" s="194">
+        <v>1</v>
+      </c>
+      <c r="F286" s="193">
+        <f t="shared" si="14"/>
+        <v>16.989999999999998</v>
+      </c>
+      <c r="G286" s="195"/>
+      <c r="H286" s="196" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A287" s="250"/>
-      <c r="B287" s="198" t="s">
-        <v>389</v>
-      </c>
-      <c r="C287" s="185" t="s">
-        <v>390</v>
-      </c>
-      <c r="D287" s="186">
-        <v>3000</v>
-      </c>
-      <c r="E287" s="185">
-        <v>1</v>
-      </c>
-      <c r="F287" s="186">
-        <f t="shared" si="13"/>
-        <v>3000</v>
-      </c>
-      <c r="G287" s="187"/>
-      <c r="H287" s="152" t="s">
-        <v>393</v>
-      </c>
+      <c r="B287" s="28"/>
+      <c r="C287" s="29"/>
+      <c r="D287" s="52"/>
+      <c r="E287" s="53"/>
+      <c r="F287" s="52"/>
+      <c r="G287" s="54"/>
+      <c r="H287" s="55"/>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A288" s="250"/>
       <c r="B288" s="198" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C288" s="185" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D288" s="186">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="E288" s="185">
         <v>1</v>
       </c>
       <c r="F288" s="186">
-        <f t="shared" si="13"/>
-        <v>2500</v>
+        <f t="shared" si="14"/>
+        <v>3000</v>
       </c>
       <c r="G288" s="187"/>
-      <c r="H288" s="190" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="289" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H288" s="152" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A289" s="250"/>
       <c r="B289" s="198" t="s">
-        <v>590</v>
-      </c>
-      <c r="C289" s="219" t="s">
-        <v>584</v>
-      </c>
-      <c r="D289" s="220"/>
-      <c r="E289" s="219">
-        <v>1</v>
-      </c>
-      <c r="F289" s="193">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G289" s="221"/>
-      <c r="H289" s="222" t="s">
-        <v>582</v>
+        <v>391</v>
+      </c>
+      <c r="C289" s="185" t="s">
+        <v>392</v>
+      </c>
+      <c r="D289" s="186">
+        <v>2500</v>
+      </c>
+      <c r="E289" s="185">
+        <v>1</v>
+      </c>
+      <c r="F289" s="186">
+        <f t="shared" si="14"/>
+        <v>2500</v>
+      </c>
+      <c r="G289" s="187"/>
+      <c r="H289" s="190" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="290" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A290" s="250"/>
       <c r="B290" s="198" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C290" s="219" t="s">
-        <v>583</v>
-      </c>
-      <c r="D290" s="220">
-        <v>34.99</v>
-      </c>
+        <v>579</v>
+      </c>
+      <c r="D290" s="220"/>
       <c r="E290" s="219">
         <v>1</v>
       </c>
       <c r="F290" s="193">
-        <f t="shared" si="13"/>
-        <v>34.99</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="G290" s="221"/>
       <c r="H290" s="222" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
     </row>
     <row r="291" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A291" s="250"/>
       <c r="B291" s="198" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C291" s="219" t="s">
-        <v>585</v>
-      </c>
-      <c r="D291" s="220"/>
+        <v>578</v>
+      </c>
+      <c r="D291" s="220">
+        <v>34.99</v>
+      </c>
       <c r="E291" s="219">
         <v>1</v>
       </c>
       <c r="F291" s="193">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>34.99</v>
       </c>
       <c r="G291" s="221"/>
       <c r="H291" s="222" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="292" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A292" s="250"/>
-      <c r="B292" s="191" t="s">
-        <v>244</v>
-      </c>
-      <c r="C292" s="192" t="s">
-        <v>245</v>
-      </c>
-      <c r="D292" s="193">
-        <v>990</v>
-      </c>
-      <c r="E292" s="194">
+      <c r="B292" s="198" t="s">
+        <v>584</v>
+      </c>
+      <c r="C292" s="219" t="s">
+        <v>580</v>
+      </c>
+      <c r="D292" s="220"/>
+      <c r="E292" s="219">
         <v>1</v>
       </c>
       <c r="F292" s="193">
-        <f t="shared" si="13"/>
-        <v>990</v>
-      </c>
-      <c r="G292" s="195"/>
-      <c r="H292" s="196" t="s">
-        <v>246</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G292" s="221"/>
+      <c r="H292" s="222" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="293" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A293" s="250"/>
       <c r="B293" s="191" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C293" s="192" t="s">
-        <v>455</v>
+        <v>245</v>
       </c>
       <c r="D293" s="193">
-        <v>360</v>
+        <v>990</v>
       </c>
       <c r="E293" s="194">
         <v>1</v>
       </c>
       <c r="F293" s="193">
-        <f t="shared" si="13"/>
-        <v>360</v>
+        <f t="shared" si="14"/>
+        <v>990</v>
       </c>
       <c r="G293" s="195"/>
       <c r="H293" s="196" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="294" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A294" s="250"/>
       <c r="B294" s="191" t="s">
-        <v>456</v>
+        <v>247</v>
       </c>
       <c r="C294" s="192" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D294" s="193">
-        <v>65</v>
+        <v>360</v>
       </c>
       <c r="E294" s="194">
         <v>1</v>
       </c>
       <c r="F294" s="193">
-        <f t="shared" si="13"/>
-        <v>65</v>
+        <f t="shared" si="14"/>
+        <v>360</v>
       </c>
       <c r="G294" s="195"/>
-      <c r="H294" s="197" t="s">
-        <v>249</v>
+      <c r="H294" s="196" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="295" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A295" s="250"/>
-      <c r="B295" s="33"/>
-      <c r="C295" s="33"/>
-      <c r="D295" s="57"/>
-      <c r="E295" s="58"/>
-      <c r="F295" s="57"/>
-      <c r="G295" s="59"/>
-      <c r="H295" s="60"/>
+      <c r="B295" s="191" t="s">
+        <v>456</v>
+      </c>
+      <c r="C295" s="192" t="s">
+        <v>454</v>
+      </c>
+      <c r="D295" s="193">
+        <v>65</v>
+      </c>
+      <c r="E295" s="194">
+        <v>1</v>
+      </c>
+      <c r="F295" s="193">
+        <f t="shared" si="14"/>
+        <v>65</v>
+      </c>
+      <c r="G295" s="195"/>
+      <c r="H295" s="197" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="296" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A296" s="250"/>
-      <c r="B296" s="36"/>
-      <c r="C296" s="36"/>
-      <c r="D296" s="61"/>
-      <c r="E296" s="62"/>
-      <c r="F296" s="63" t="s">
+      <c r="B296" s="33"/>
+      <c r="C296" s="33"/>
+      <c r="D296" s="57"/>
+      <c r="E296" s="58"/>
+      <c r="F296" s="57"/>
+      <c r="G296" s="59"/>
+      <c r="H296" s="60"/>
+    </row>
+    <row r="297" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A297" s="250"/>
+      <c r="B297" s="36"/>
+      <c r="C297" s="36"/>
+      <c r="D297" s="61"/>
+      <c r="E297" s="62"/>
+      <c r="F297" s="63" t="s">
         <v>250</v>
       </c>
-      <c r="G296" s="64">
-        <f>SUM(F276:F294)</f>
+      <c r="G297" s="64">
+        <f>SUM(F277:F295)</f>
         <v>8658.01</v>
       </c>
-      <c r="H296" s="65"/>
-    </row>
-    <row r="297" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A297" s="39"/>
-      <c r="B297" s="39"/>
-      <c r="C297" s="39"/>
-      <c r="D297" s="66"/>
-      <c r="E297" s="67"/>
-      <c r="F297" s="66"/>
-      <c r="G297" s="68"/>
-      <c r="H297" s="67"/>
-    </row>
-    <row r="298" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A298" s="250" t="s">
+      <c r="H297" s="65"/>
+    </row>
+    <row r="298" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A298" s="39"/>
+      <c r="B298" s="39"/>
+      <c r="C298" s="39"/>
+      <c r="D298" s="66"/>
+      <c r="E298" s="67"/>
+      <c r="F298" s="66"/>
+      <c r="G298" s="68"/>
+      <c r="H298" s="67"/>
+    </row>
+    <row r="299" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A299" s="250" t="s">
         <v>251</v>
       </c>
-      <c r="B298" s="69" t="s">
+      <c r="B299" s="69" t="s">
         <v>252</v>
-      </c>
-      <c r="C298" s="70"/>
-      <c r="D298" s="31">
-        <v>107.47</v>
-      </c>
-      <c r="E298" s="70">
-        <v>1</v>
-      </c>
-      <c r="F298" s="31">
-        <f t="shared" ref="F298" si="14">D298*E298</f>
-        <v>107.47</v>
-      </c>
-      <c r="G298" s="70"/>
-      <c r="H298" s="71" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A299" s="250"/>
-      <c r="B299" s="69" t="s">
-        <v>254</v>
       </c>
       <c r="C299" s="70"/>
       <c r="D299" s="31">
-        <v>5.67</v>
+        <v>107.47</v>
       </c>
       <c r="E299" s="70">
         <v>1</v>
       </c>
       <c r="F299" s="31">
-        <f t="shared" ref="F299:F308" si="15">D299*E299</f>
-        <v>5.67</v>
-      </c>
-      <c r="G299" s="72"/>
+        <f t="shared" ref="F299" si="15">D299*E299</f>
+        <v>107.47</v>
+      </c>
+      <c r="G299" s="70"/>
       <c r="H299" s="71" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A300" s="250"/>
       <c r="B300" s="69" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C300" s="70"/>
       <c r="D300" s="31">
@@ -9342,102 +9355,102 @@
         <v>1</v>
       </c>
       <c r="F300" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="F300:F309" si="16">D300*E300</f>
         <v>5.67</v>
       </c>
       <c r="G300" s="72"/>
       <c r="H300" s="71" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A301" s="250"/>
       <c r="B301" s="69" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C301" s="70"/>
       <c r="D301" s="31">
-        <v>6.47</v>
+        <v>5.67</v>
       </c>
       <c r="E301" s="70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F301" s="31">
-        <f t="shared" si="15"/>
-        <v>12.94</v>
+        <f t="shared" si="16"/>
+        <v>5.67</v>
       </c>
       <c r="G301" s="72"/>
       <c r="H301" s="71" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A302" s="250"/>
       <c r="B302" s="69" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C302" s="70"/>
       <c r="D302" s="31">
-        <v>34.950000000000003</v>
+        <v>6.47</v>
       </c>
       <c r="E302" s="70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F302" s="31">
-        <f t="shared" si="15"/>
-        <v>34.950000000000003</v>
+        <f t="shared" si="16"/>
+        <v>12.94</v>
       </c>
       <c r="G302" s="72"/>
       <c r="H302" s="71" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A303" s="250"/>
       <c r="B303" s="69" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C303" s="70"/>
       <c r="D303" s="31">
-        <v>3.95</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="E303" s="70">
         <v>1</v>
       </c>
       <c r="F303" s="31">
-        <f t="shared" si="15"/>
-        <v>3.95</v>
+        <f t="shared" si="16"/>
+        <v>34.950000000000003</v>
       </c>
       <c r="G303" s="72"/>
       <c r="H303" s="71" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A304" s="250"/>
       <c r="B304" s="69" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C304" s="70"/>
       <c r="D304" s="31">
-        <v>6.95</v>
+        <v>3.95</v>
       </c>
       <c r="E304" s="70">
         <v>1</v>
       </c>
       <c r="F304" s="31">
-        <f t="shared" si="15"/>
-        <v>6.95</v>
+        <f t="shared" si="16"/>
+        <v>3.95</v>
       </c>
       <c r="G304" s="72"/>
       <c r="H304" s="71" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A305" s="250"/>
       <c r="B305" s="69" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C305" s="70"/>
       <c r="D305" s="31">
@@ -9447,39 +9460,39 @@
         <v>1</v>
       </c>
       <c r="F305" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6.95</v>
       </c>
       <c r="G305" s="72"/>
       <c r="H305" s="71" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A306" s="250"/>
       <c r="B306" s="69" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C306" s="70"/>
       <c r="D306" s="31">
-        <v>3.99</v>
+        <v>6.95</v>
       </c>
       <c r="E306" s="70">
         <v>1</v>
       </c>
       <c r="F306" s="31">
-        <f t="shared" si="15"/>
-        <v>3.99</v>
+        <f t="shared" si="16"/>
+        <v>6.95</v>
       </c>
       <c r="G306" s="72"/>
       <c r="H306" s="71" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A307" s="250"/>
       <c r="B307" s="69" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C307" s="70"/>
       <c r="D307" s="31">
@@ -9489,789 +9502,810 @@
         <v>1</v>
       </c>
       <c r="F307" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.99</v>
       </c>
       <c r="G307" s="72"/>
       <c r="H307" s="71" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A308" s="250"/>
       <c r="B308" s="69" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C308" s="70"/>
       <c r="D308" s="31">
-        <v>10.87</v>
+        <v>3.99</v>
       </c>
       <c r="E308" s="70">
         <v>1</v>
       </c>
       <c r="F308" s="31">
-        <f t="shared" si="15"/>
-        <v>10.87</v>
+        <f t="shared" si="16"/>
+        <v>3.99</v>
       </c>
       <c r="G308" s="72"/>
       <c r="H308" s="71" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A309" s="250"/>
-      <c r="B309" s="167"/>
-      <c r="C309" s="168"/>
-      <c r="D309" s="169"/>
-      <c r="E309" s="168"/>
-      <c r="F309" s="169"/>
-      <c r="G309" s="170"/>
-      <c r="H309" s="171"/>
+      <c r="B309" s="69" t="s">
+        <v>272</v>
+      </c>
+      <c r="C309" s="70"/>
+      <c r="D309" s="31">
+        <v>10.87</v>
+      </c>
+      <c r="E309" s="70">
+        <v>1</v>
+      </c>
+      <c r="F309" s="31">
+        <f t="shared" si="16"/>
+        <v>10.87</v>
+      </c>
+      <c r="G309" s="72"/>
+      <c r="H309" s="71" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A310" s="251"/>
-      <c r="B310" s="162" t="s">
+      <c r="A310" s="250"/>
+      <c r="B310" s="167"/>
+      <c r="C310" s="168"/>
+      <c r="D310" s="169"/>
+      <c r="E310" s="168"/>
+      <c r="F310" s="169"/>
+      <c r="G310" s="170"/>
+      <c r="H310" s="171"/>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A311" s="251"/>
+      <c r="B311" s="162" t="s">
         <v>428</v>
       </c>
-      <c r="C310" s="163"/>
-      <c r="D310" s="31">
+      <c r="C311" s="163"/>
+      <c r="D311" s="31">
         <v>65.59</v>
       </c>
-      <c r="E310" s="164">
-        <v>1</v>
-      </c>
-      <c r="F310" s="91">
-        <f t="shared" ref="F310:F336" si="16">D310*E310</f>
+      <c r="E311" s="164">
+        <v>1</v>
+      </c>
+      <c r="F311" s="91">
+        <f t="shared" ref="F311:F337" si="17">D311*E311</f>
         <v>65.59</v>
       </c>
-      <c r="G310" s="163"/>
-      <c r="H310" s="165" t="s">
+      <c r="G311" s="163"/>
+      <c r="H311" s="165" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A311" s="250"/>
-      <c r="B311" s="172" t="s">
-        <v>274</v>
-      </c>
-      <c r="C311" s="173"/>
-      <c r="D311" s="153">
-        <v>34.69</v>
-      </c>
-      <c r="E311" s="173">
-        <v>1</v>
-      </c>
-      <c r="F311" s="153">
-        <f t="shared" si="16"/>
-        <v>34.69</v>
-      </c>
-      <c r="G311" s="174"/>
-      <c r="H311" s="175" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A312" s="250"/>
-      <c r="B312" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="C312" s="70"/>
-      <c r="D312" s="31">
-        <v>10.29</v>
-      </c>
-      <c r="E312" s="70">
-        <v>1</v>
-      </c>
-      <c r="F312" s="31">
-        <f t="shared" si="16"/>
-        <v>10.29</v>
-      </c>
-      <c r="G312" s="72"/>
-      <c r="H312" s="71" t="s">
-        <v>277</v>
+      <c r="B312" s="172" t="s">
+        <v>274</v>
+      </c>
+      <c r="C312" s="173"/>
+      <c r="D312" s="153">
+        <v>34.69</v>
+      </c>
+      <c r="E312" s="173">
+        <v>1</v>
+      </c>
+      <c r="F312" s="153">
+        <f t="shared" si="17"/>
+        <v>34.69</v>
+      </c>
+      <c r="G312" s="174"/>
+      <c r="H312" s="175" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A313" s="250"/>
       <c r="B313" s="69" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C313" s="70"/>
       <c r="D313" s="31">
-        <v>3.96</v>
+        <v>10.29</v>
       </c>
       <c r="E313" s="70">
         <v>1</v>
       </c>
       <c r="F313" s="31">
-        <f t="shared" si="16"/>
-        <v>3.96</v>
+        <f t="shared" si="17"/>
+        <v>10.29</v>
       </c>
       <c r="G313" s="72"/>
       <c r="H313" s="71" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A314" s="250"/>
       <c r="B314" s="69" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C314" s="70"/>
       <c r="D314" s="31">
-        <v>3.44</v>
+        <v>3.96</v>
       </c>
       <c r="E314" s="70">
         <v>1</v>
       </c>
       <c r="F314" s="31">
-        <f t="shared" si="16"/>
-        <v>3.44</v>
+        <f t="shared" si="17"/>
+        <v>3.96</v>
       </c>
       <c r="G314" s="72"/>
       <c r="H314" s="71" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A315" s="250"/>
       <c r="B315" s="69" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C315" s="70"/>
       <c r="D315" s="31">
-        <v>3.27</v>
+        <v>3.44</v>
       </c>
       <c r="E315" s="70">
         <v>1</v>
       </c>
       <c r="F315" s="31">
-        <f t="shared" si="16"/>
-        <v>3.27</v>
+        <f t="shared" si="17"/>
+        <v>3.44</v>
       </c>
       <c r="G315" s="72"/>
       <c r="H315" s="71" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A316" s="250"/>
       <c r="B316" s="69" t="s">
-        <v>431</v>
+        <v>282</v>
       </c>
       <c r="C316" s="70"/>
       <c r="D316" s="31">
-        <v>5.46</v>
+        <v>3.27</v>
       </c>
       <c r="E316" s="70">
         <v>1</v>
       </c>
       <c r="F316" s="31">
-        <f t="shared" si="16"/>
-        <v>5.46</v>
+        <f t="shared" si="17"/>
+        <v>3.27</v>
       </c>
       <c r="G316" s="72"/>
       <c r="H316" s="71" t="s">
-        <v>430</v>
+        <v>283</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A317" s="250"/>
       <c r="B317" s="69" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C317" s="70"/>
       <c r="D317" s="31">
-        <v>5.64</v>
+        <v>5.46</v>
       </c>
       <c r="E317" s="70">
         <v>1</v>
       </c>
       <c r="F317" s="31">
-        <f t="shared" si="16"/>
-        <v>5.64</v>
+        <f t="shared" si="17"/>
+        <v>5.46</v>
       </c>
       <c r="G317" s="72"/>
       <c r="H317" s="71" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A318" s="250"/>
       <c r="B318" s="69" t="s">
-        <v>284</v>
+        <v>432</v>
       </c>
       <c r="C318" s="70"/>
       <c r="D318" s="31">
-        <v>6.48</v>
+        <v>5.64</v>
       </c>
       <c r="E318" s="70">
         <v>1</v>
       </c>
       <c r="F318" s="31">
-        <f t="shared" si="16"/>
-        <v>6.48</v>
+        <f t="shared" si="17"/>
+        <v>5.64</v>
       </c>
       <c r="G318" s="72"/>
       <c r="H318" s="71" t="s">
-        <v>285</v>
+        <v>433</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A319" s="250"/>
       <c r="B319" s="69" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C319" s="70"/>
       <c r="D319" s="31">
-        <v>9.3000000000000007</v>
+        <v>6.48</v>
       </c>
       <c r="E319" s="70">
         <v>1</v>
       </c>
       <c r="F319" s="31">
-        <f t="shared" si="16"/>
-        <v>9.3000000000000007</v>
+        <f t="shared" si="17"/>
+        <v>6.48</v>
       </c>
       <c r="G319" s="72"/>
       <c r="H319" s="71" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A320" s="250"/>
       <c r="B320" s="69" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C320" s="70"/>
       <c r="D320" s="31">
-        <v>18.649999999999999</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E320" s="70">
         <v>1</v>
       </c>
       <c r="F320" s="31">
-        <f t="shared" si="16"/>
-        <v>18.649999999999999</v>
+        <f t="shared" si="17"/>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G320" s="72"/>
       <c r="H320" s="71" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A321" s="250"/>
       <c r="B321" s="69" t="s">
-        <v>506</v>
+        <v>288</v>
       </c>
       <c r="C321" s="70"/>
       <c r="D321" s="31">
-        <v>6.85</v>
+        <v>18.649999999999999</v>
       </c>
       <c r="E321" s="70">
         <v>1</v>
       </c>
       <c r="F321" s="31">
-        <f t="shared" si="16"/>
-        <v>6.85</v>
+        <f t="shared" si="17"/>
+        <v>18.649999999999999</v>
       </c>
       <c r="G321" s="72"/>
       <c r="H321" s="71" t="s">
-        <v>507</v>
+        <v>289</v>
       </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A322" s="250"/>
       <c r="B322" s="69" t="s">
-        <v>290</v>
+        <v>502</v>
       </c>
       <c r="C322" s="70"/>
       <c r="D322" s="31">
-        <v>21.84</v>
+        <v>6.85</v>
       </c>
       <c r="E322" s="70">
         <v>1</v>
       </c>
       <c r="F322" s="31">
-        <f t="shared" si="16"/>
-        <v>21.84</v>
+        <f t="shared" si="17"/>
+        <v>6.85</v>
       </c>
       <c r="G322" s="72"/>
       <c r="H322" s="71" t="s">
-        <v>291</v>
+        <v>503</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A323" s="250"/>
       <c r="B323" s="69" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C323" s="70"/>
       <c r="D323" s="31">
-        <v>17.5</v>
+        <v>21.84</v>
       </c>
       <c r="E323" s="70">
         <v>1</v>
       </c>
       <c r="F323" s="31">
-        <f t="shared" si="16"/>
-        <v>17.5</v>
+        <f t="shared" si="17"/>
+        <v>21.84</v>
       </c>
       <c r="G323" s="72"/>
       <c r="H323" s="71" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A324" s="250"/>
       <c r="B324" s="69" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C324" s="70"/>
       <c r="D324" s="31">
-        <v>19.64</v>
+        <v>17.5</v>
       </c>
       <c r="E324" s="70">
         <v>1</v>
       </c>
       <c r="F324" s="31">
-        <f t="shared" si="16"/>
-        <v>19.64</v>
-      </c>
-      <c r="G324" s="70"/>
+        <f t="shared" si="17"/>
+        <v>17.5</v>
+      </c>
+      <c r="G324" s="72"/>
       <c r="H324" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A325" s="250"/>
       <c r="B325" s="69" t="s">
-        <v>560</v>
+        <v>294</v>
       </c>
       <c r="C325" s="70"/>
       <c r="D325" s="31">
-        <v>18.47</v>
+        <v>19.64</v>
       </c>
       <c r="E325" s="70">
         <v>1</v>
       </c>
       <c r="F325" s="31">
-        <f t="shared" si="16"/>
-        <v>18.47</v>
+        <f t="shared" si="17"/>
+        <v>19.64</v>
       </c>
       <c r="G325" s="70"/>
       <c r="H325" s="71" t="s">
-        <v>434</v>
+        <v>295</v>
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A326" s="250"/>
       <c r="B326" s="69" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C326" s="70"/>
       <c r="D326" s="31">
-        <v>16.48</v>
+        <v>18.47</v>
       </c>
       <c r="E326" s="70">
         <v>1</v>
       </c>
       <c r="F326" s="31">
-        <f t="shared" si="16"/>
-        <v>16.48</v>
+        <f t="shared" si="17"/>
+        <v>18.47</v>
       </c>
       <c r="G326" s="70"/>
       <c r="H326" s="71" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A327" s="250"/>
       <c r="B327" s="69" t="s">
-        <v>445</v>
+        <v>554</v>
       </c>
       <c r="C327" s="70"/>
       <c r="D327" s="31">
-        <v>2.29</v>
+        <v>16.48</v>
       </c>
       <c r="E327" s="70">
         <v>1</v>
       </c>
       <c r="F327" s="31">
-        <f t="shared" si="16"/>
-        <v>2.29</v>
+        <f t="shared" si="17"/>
+        <v>16.48</v>
       </c>
       <c r="G327" s="70"/>
       <c r="H327" s="71" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A328" s="250"/>
       <c r="B328" s="69" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="C328" s="70"/>
       <c r="D328" s="31">
-        <v>3.34</v>
+        <v>2.29</v>
       </c>
       <c r="E328" s="70">
         <v>1</v>
       </c>
       <c r="F328" s="31">
-        <f t="shared" si="16"/>
-        <v>3.34</v>
+        <f t="shared" si="17"/>
+        <v>2.29</v>
       </c>
       <c r="G328" s="70"/>
       <c r="H328" s="71" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A329" s="250"/>
       <c r="B329" s="69" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C329" s="70"/>
       <c r="D329" s="31">
-        <v>3.45</v>
+        <v>3.34</v>
       </c>
       <c r="E329" s="70">
         <v>1</v>
       </c>
       <c r="F329" s="31">
-        <f t="shared" si="16"/>
-        <v>3.45</v>
+        <f t="shared" si="17"/>
+        <v>3.34</v>
       </c>
       <c r="G329" s="70"/>
       <c r="H329" s="71" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A330" s="250"/>
       <c r="B330" s="69" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C330" s="70"/>
       <c r="D330" s="31">
-        <v>6.16</v>
+        <v>3.45</v>
       </c>
       <c r="E330" s="70">
         <v>1</v>
       </c>
       <c r="F330" s="31">
-        <f t="shared" si="16"/>
-        <v>6.16</v>
+        <f t="shared" si="17"/>
+        <v>3.45</v>
       </c>
       <c r="G330" s="70"/>
       <c r="H330" s="71" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A331" s="250"/>
       <c r="B331" s="69" t="s">
-        <v>558</v>
+        <v>437</v>
       </c>
       <c r="C331" s="70"/>
       <c r="D331" s="31">
-        <v>3.2</v>
+        <v>6.16</v>
       </c>
       <c r="E331" s="70">
         <v>1</v>
       </c>
       <c r="F331" s="31">
-        <f t="shared" si="16"/>
-        <v>3.2</v>
+        <f t="shared" si="17"/>
+        <v>6.16</v>
       </c>
       <c r="G331" s="70"/>
       <c r="H331" s="71" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A332" s="250"/>
       <c r="B332" s="69" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C332" s="70"/>
       <c r="D332" s="31">
-        <v>3.44</v>
+        <v>3.2</v>
       </c>
       <c r="E332" s="70">
         <v>1</v>
       </c>
       <c r="F332" s="31">
-        <f t="shared" si="16"/>
-        <v>3.44</v>
+        <f t="shared" si="17"/>
+        <v>3.2</v>
       </c>
       <c r="G332" s="70"/>
       <c r="H332" s="71" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A333" s="250"/>
       <c r="B333" s="69" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C333" s="70"/>
       <c r="D333" s="31">
-        <v>5.1100000000000003</v>
+        <v>3.44</v>
       </c>
       <c r="E333" s="70">
         <v>1</v>
       </c>
       <c r="F333" s="31">
-        <f t="shared" si="16"/>
-        <v>5.1100000000000003</v>
+        <f t="shared" si="17"/>
+        <v>3.44</v>
       </c>
       <c r="G333" s="70"/>
       <c r="H333" s="71" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A334" s="250"/>
-      <c r="B334" s="69"/>
+      <c r="B334" s="69" t="s">
+        <v>551</v>
+      </c>
       <c r="C334" s="70"/>
-      <c r="D334" s="31"/>
-      <c r="E334" s="70"/>
-      <c r="F334" s="31"/>
+      <c r="D334" s="31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E334" s="70">
+        <v>1</v>
+      </c>
+      <c r="F334" s="31">
+        <f t="shared" si="17"/>
+        <v>5.1100000000000003</v>
+      </c>
       <c r="G334" s="70"/>
-      <c r="H334" s="73"/>
+      <c r="H334" s="71" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A335" s="250"/>
-      <c r="B335" s="69" t="s">
-        <v>529</v>
-      </c>
+      <c r="B335" s="69"/>
       <c r="C335" s="70"/>
-      <c r="D335" s="31">
-        <v>39.99</v>
-      </c>
-      <c r="E335" s="70">
-        <v>1</v>
-      </c>
-      <c r="F335" s="31">
-        <f t="shared" si="16"/>
-        <v>39.99</v>
-      </c>
+      <c r="D335" s="31"/>
+      <c r="E335" s="70"/>
+      <c r="F335" s="31"/>
       <c r="G335" s="70"/>
-      <c r="H335" s="152" t="s">
-        <v>497</v>
-      </c>
+      <c r="H335" s="73"/>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A336" s="250"/>
       <c r="B336" s="69" t="s">
-        <v>495</v>
+        <v>524</v>
       </c>
       <c r="C336" s="70"/>
       <c r="D336" s="31">
-        <v>7.99</v>
+        <v>39.99</v>
       </c>
       <c r="E336" s="70">
         <v>1</v>
       </c>
       <c r="F336" s="31">
-        <f t="shared" si="16"/>
-        <v>7.99</v>
+        <f t="shared" si="17"/>
+        <v>39.99</v>
       </c>
       <c r="G336" s="70"/>
       <c r="H336" s="152" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A337" s="250"/>
-      <c r="B337" s="69"/>
+      <c r="B337" s="69" t="s">
+        <v>491</v>
+      </c>
       <c r="C337" s="70"/>
-      <c r="D337" s="31"/>
-      <c r="E337" s="70"/>
-      <c r="F337" s="31"/>
+      <c r="D337" s="31">
+        <v>7.99</v>
+      </c>
+      <c r="E337" s="70">
+        <v>1</v>
+      </c>
+      <c r="F337" s="31">
+        <f t="shared" si="17"/>
+        <v>7.99</v>
+      </c>
       <c r="G337" s="70"/>
-      <c r="H337" s="73"/>
+      <c r="H337" s="152" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A338" s="250"/>
-      <c r="B338" s="69" t="s">
-        <v>296</v>
-      </c>
+      <c r="B338" s="69"/>
       <c r="C338" s="70"/>
-      <c r="D338" s="31">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E338" s="70">
-        <v>1</v>
-      </c>
-      <c r="F338" s="31">
-        <f>D338*E338</f>
-        <v>18.600000000000001</v>
-      </c>
+      <c r="D338" s="31"/>
+      <c r="E338" s="70"/>
+      <c r="F338" s="31"/>
       <c r="G338" s="70"/>
-      <c r="H338" s="71" t="s">
-        <v>297</v>
-      </c>
+      <c r="H338" s="73"/>
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A339" s="250"/>
-      <c r="B339" s="69"/>
+      <c r="B339" s="69" t="s">
+        <v>296</v>
+      </c>
       <c r="C339" s="70"/>
-      <c r="D339" s="31"/>
-      <c r="E339" s="70"/>
-      <c r="F339" s="31"/>
+      <c r="D339" s="31">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E339" s="70">
+        <v>1</v>
+      </c>
+      <c r="F339" s="31">
+        <f>D339*E339</f>
+        <v>18.600000000000001</v>
+      </c>
       <c r="G339" s="70"/>
-      <c r="H339" s="71"/>
-    </row>
-    <row r="340" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H339" s="71" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A340" s="250"/>
-      <c r="B340" s="69" t="s">
-        <v>447</v>
-      </c>
+      <c r="B340" s="69"/>
       <c r="C340" s="70"/>
-      <c r="D340" s="31">
-        <v>7.33</v>
-      </c>
-      <c r="E340" s="70">
-        <v>1</v>
-      </c>
-      <c r="F340" s="31">
-        <f t="shared" ref="F340:F343" si="17">D340*E340</f>
-        <v>7.33</v>
-      </c>
+      <c r="D340" s="31"/>
+      <c r="E340" s="70"/>
+      <c r="F340" s="31"/>
       <c r="G340" s="70"/>
-      <c r="H340" s="71" t="s">
-        <v>448</v>
-      </c>
+      <c r="H340" s="71"/>
     </row>
     <row r="341" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A341" s="250"/>
       <c r="B341" s="69" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C341" s="70"/>
       <c r="D341" s="31">
-        <v>3.7</v>
+        <v>7.33</v>
       </c>
       <c r="E341" s="70">
         <v>1</v>
       </c>
       <c r="F341" s="31">
-        <f t="shared" si="17"/>
-        <v>3.7</v>
+        <f t="shared" ref="F341:F344" si="18">D341*E341</f>
+        <v>7.33</v>
       </c>
       <c r="G341" s="70"/>
       <c r="H341" s="71" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A342" s="250"/>
       <c r="B342" s="69" t="s">
-        <v>425</v>
-      </c>
-      <c r="C342" s="70" t="s">
-        <v>426</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="C342" s="70"/>
       <c r="D342" s="31">
-        <v>162</v>
+        <v>3.7</v>
       </c>
       <c r="E342" s="70">
         <v>1</v>
       </c>
       <c r="F342" s="31">
-        <f t="shared" si="17"/>
-        <v>162</v>
+        <f t="shared" si="18"/>
+        <v>3.7</v>
       </c>
       <c r="G342" s="70"/>
       <c r="H342" s="71" t="s">
-        <v>427</v>
+        <v>450</v>
       </c>
     </row>
     <row r="343" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A343" s="250"/>
-      <c r="B343" s="28" t="s">
-        <v>505</v>
-      </c>
-      <c r="C343" s="29" t="s">
-        <v>492</v>
-      </c>
-      <c r="D343" s="30">
-        <v>24.85</v>
-      </c>
-      <c r="E343" s="29">
+      <c r="B343" s="69" t="s">
+        <v>425</v>
+      </c>
+      <c r="C343" s="70" t="s">
+        <v>426</v>
+      </c>
+      <c r="D343" s="31">
+        <v>162</v>
+      </c>
+      <c r="E343" s="70">
         <v>1</v>
       </c>
       <c r="F343" s="31">
-        <f t="shared" si="17"/>
-        <v>24.85</v>
-      </c>
-      <c r="G343" s="29"/>
-      <c r="H343" s="149" t="s">
-        <v>493</v>
+        <f t="shared" si="18"/>
+        <v>162</v>
+      </c>
+      <c r="G343" s="70"/>
+      <c r="H343" s="71" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="344" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A344" s="250"/>
       <c r="B344" s="28" t="s">
-        <v>503</v>
-      </c>
-      <c r="C344" s="29"/>
+        <v>501</v>
+      </c>
+      <c r="C344" s="29" t="s">
+        <v>489</v>
+      </c>
       <c r="D344" s="30">
-        <v>18.68</v>
+        <v>24.85</v>
       </c>
       <c r="E344" s="29">
         <v>1</v>
       </c>
       <c r="F344" s="31">
-        <v>18.68</v>
+        <f t="shared" si="18"/>
+        <v>24.85</v>
       </c>
       <c r="G344" s="29"/>
       <c r="H344" s="149" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
     </row>
     <row r="345" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A345" s="250"/>
-      <c r="B345" s="33"/>
-      <c r="C345" s="33"/>
-      <c r="D345" s="34"/>
-      <c r="E345" s="33"/>
-      <c r="F345" s="153"/>
-      <c r="G345" s="33"/>
-      <c r="H345" s="42"/>
+      <c r="B345" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="C345" s="29"/>
+      <c r="D345" s="30">
+        <v>18.68</v>
+      </c>
+      <c r="E345" s="29">
+        <v>1</v>
+      </c>
+      <c r="F345" s="31">
+        <v>18.68</v>
+      </c>
+      <c r="G345" s="29"/>
+      <c r="H345" s="149" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="346" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A346" s="250"/>
-      <c r="B346" s="36"/>
-      <c r="C346" s="36"/>
-      <c r="D346" s="36"/>
-      <c r="E346" s="36"/>
-      <c r="F346" s="28" t="s">
+      <c r="B346" s="33"/>
+      <c r="C346" s="33"/>
+      <c r="D346" s="34"/>
+      <c r="E346" s="33"/>
+      <c r="F346" s="153"/>
+      <c r="G346" s="33"/>
+      <c r="H346" s="42"/>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A347" s="250"/>
+      <c r="B347" s="36"/>
+      <c r="C347" s="36"/>
+      <c r="D347" s="36"/>
+      <c r="E347" s="36"/>
+      <c r="F347" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="G346" s="200">
-        <f>SUM(F298:F344)</f>
+      <c r="G347" s="200">
+        <f>SUM(F299:F345)</f>
         <v>781.08</v>
       </c>
-      <c r="H346" s="38"/>
+      <c r="H347" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A267:B267"/>
-    <mergeCell ref="A272:H272"/>
+    <mergeCell ref="A268:B268"/>
     <mergeCell ref="A273:H273"/>
-    <mergeCell ref="A276:A296"/>
-    <mergeCell ref="A298:A346"/>
-    <mergeCell ref="F267:G267"/>
     <mergeCell ref="A274:H274"/>
+    <mergeCell ref="A277:A297"/>
+    <mergeCell ref="A299:A347"/>
+    <mergeCell ref="F268:G268"/>
+    <mergeCell ref="A275:H275"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A19:A126"/>
     <mergeCell ref="A128:A180"/>
-    <mergeCell ref="A183:A262"/>
+    <mergeCell ref="A183:A263"/>
     <mergeCell ref="B216:C216"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
@@ -10282,88 +10316,88 @@
     <mergeCell ref="A4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H25" r:id="rId1"/>
-    <hyperlink ref="H28" r:id="rId2"/>
-    <hyperlink ref="H34" r:id="rId3"/>
-    <hyperlink ref="H35" r:id="rId4"/>
-    <hyperlink ref="H46" r:id="rId5"/>
-    <hyperlink ref="H71" r:id="rId6" location="92290a474/=120dvtd"/>
-    <hyperlink ref="H72" r:id="rId7" location="91828a005/=120dvjk"/>
-    <hyperlink ref="H73" r:id="rId8" location="95610a530/=120dwf7"/>
-    <hyperlink ref="H77" r:id="rId9" location="90591a250/=120dy5e"/>
-    <hyperlink ref="H81" r:id="rId10" location="91290a113/=120e123"/>
-    <hyperlink ref="H83" r:id="rId11" location="91290a117/=120e45y"/>
-    <hyperlink ref="H84" r:id="rId12" location="91290a120/=120epou"/>
-    <hyperlink ref="H89" r:id="rId13" location="91290a137/=120e644"/>
-    <hyperlink ref="H90" r:id="rId14" location="92185a144/=120dvzz"/>
-    <hyperlink ref="H91" r:id="rId15" location="7840k72/=120duy7"/>
-    <hyperlink ref="H93" r:id="rId16" location="94669a041/=120elfz"/>
-    <hyperlink ref="H94" r:id="rId17" location="90591a255/=120em4k"/>
-    <hyperlink ref="H96" r:id="rId18" location="91290a150/=120enm4"/>
-    <hyperlink ref="H101" r:id="rId19" location="92390a100/=128m34x"/>
-    <hyperlink ref="H103" r:id="rId20" location="8548k23/=128m659"/>
-    <hyperlink ref="H104" r:id="rId21" location="8542k51/=128m6ms"/>
-    <hyperlink ref="H107" r:id="rId22" location="8973k68/=128m88a"/>
-    <hyperlink ref="H109" r:id="rId23" location="7130k52/=120erv8"/>
-    <hyperlink ref="H110" r:id="rId24" location="7130k104/=120evi5"/>
-    <hyperlink ref="H111" r:id="rId25" location="7566k73/=120ew2s"/>
-    <hyperlink ref="H112" r:id="rId26" location="76425a51/=120exoz"/>
-    <hyperlink ref="H113" r:id="rId27" location="76425a51/=120eyab"/>
-    <hyperlink ref="H114" r:id="rId28" location="91458a115/=120e79s"/>
-    <hyperlink ref="H143" r:id="rId29"/>
-    <hyperlink ref="H152" r:id="rId30"/>
-    <hyperlink ref="H165" r:id="rId31"/>
-    <hyperlink ref="H176" r:id="rId32"/>
-    <hyperlink ref="H177" r:id="rId33"/>
-    <hyperlink ref="H178" r:id="rId34"/>
-    <hyperlink ref="H190" r:id="rId35"/>
-    <hyperlink ref="H194" r:id="rId36"/>
-    <hyperlink ref="H202" r:id="rId37"/>
-    <hyperlink ref="H204" r:id="rId38"/>
-    <hyperlink ref="H213" r:id="rId39"/>
-    <hyperlink ref="H214" r:id="rId40"/>
-    <hyperlink ref="H215" r:id="rId41"/>
-    <hyperlink ref="H218" r:id="rId42"/>
-    <hyperlink ref="H222" r:id="rId43"/>
-    <hyperlink ref="H223" r:id="rId44"/>
-    <hyperlink ref="H224" r:id="rId45"/>
-    <hyperlink ref="H225" r:id="rId46"/>
-    <hyperlink ref="H226" r:id="rId47"/>
-    <hyperlink ref="H227" r:id="rId48"/>
-    <hyperlink ref="H228" r:id="rId49"/>
-    <hyperlink ref="H229" r:id="rId50"/>
-    <hyperlink ref="H231" r:id="rId51"/>
-    <hyperlink ref="H232" r:id="rId52"/>
-    <hyperlink ref="H233" r:id="rId53"/>
-    <hyperlink ref="H234" r:id="rId54"/>
-    <hyperlink ref="H246" r:id="rId55"/>
-    <hyperlink ref="H250" r:id="rId56"/>
-    <hyperlink ref="H251" r:id="rId57"/>
-    <hyperlink ref="H256" r:id="rId58"/>
-    <hyperlink ref="H260" r:id="rId59"/>
-    <hyperlink ref="H257" r:id="rId60"/>
-    <hyperlink ref="H298" r:id="rId61"/>
-    <hyperlink ref="H299" r:id="rId62"/>
-    <hyperlink ref="H300" r:id="rId63"/>
-    <hyperlink ref="H302" r:id="rId64"/>
-    <hyperlink ref="H131" r:id="rId65"/>
-    <hyperlink ref="H197" r:id="rId66"/>
-    <hyperlink ref="H241" r:id="rId67"/>
-    <hyperlink ref="H186" r:id="rId68"/>
-    <hyperlink ref="H187" r:id="rId69"/>
-    <hyperlink ref="H189" r:id="rId70"/>
-    <hyperlink ref="H335" r:id="rId71"/>
-    <hyperlink ref="H336" r:id="rId72"/>
-    <hyperlink ref="H343" r:id="rId73"/>
-    <hyperlink ref="H287" r:id="rId74"/>
-    <hyperlink ref="H276" r:id="rId75"/>
-    <hyperlink ref="H171" r:id="rId76"/>
-    <hyperlink ref="H172" r:id="rId77"/>
-    <hyperlink ref="H147" r:id="rId78"/>
-    <hyperlink ref="H146" r:id="rId79"/>
-    <hyperlink ref="H116" r:id="rId80"/>
-    <hyperlink ref="H65" r:id="rId81"/>
-    <hyperlink ref="H54" r:id="rId82"/>
+    <hyperlink ref="H25" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H28" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H35" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H46" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H71" r:id="rId6" location="92290a474/=120dvtd" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H72" r:id="rId7" location="91828a005/=120dvjk" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H73" r:id="rId8" location="95610a530/=120dwf7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H77" r:id="rId9" location="90591a250/=120dy5e" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H81" r:id="rId10" location="91290a113/=120e123" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H83" r:id="rId11" location="91290a117/=120e45y" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H84" r:id="rId12" location="91290a120/=120epou" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H89" r:id="rId13" location="91290a137/=120e644" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H90" r:id="rId14" location="92185a144/=120dvzz" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H91" r:id="rId15" location="7840k72/=120duy7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H93" r:id="rId16" location="94669a041/=120elfz" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H94" r:id="rId17" location="90591a255/=120em4k" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H96" r:id="rId18" location="91290a150/=120enm4" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H101" r:id="rId19" location="92390a100/=128m34x" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H103" r:id="rId20" location="8548k23/=128m659" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H104" r:id="rId21" location="8542k51/=128m6ms" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H107" r:id="rId22" location="8973k68/=128m88a" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H109" r:id="rId23" location="7130k52/=120erv8" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H110" r:id="rId24" location="7130k104/=120evi5" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H111" r:id="rId25" location="7566k73/=120ew2s" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H112" r:id="rId26" location="76425a51/=120exoz" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H113" r:id="rId27" location="76425a51/=120eyab" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H114" r:id="rId28" location="91458a115/=120e79s" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H143" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H152" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H165" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H175" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H176" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H177" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H190" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H194" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H202" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H204" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H212" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H213" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H214" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H218" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H222" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="H223" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H224" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H225" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H226" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="H227" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="H228" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="H229" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="H231" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="H232" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="H233" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="H234" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="H246" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="H250" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H251" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="H257" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="H261" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H258" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="H299" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="H300" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="H301" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="H303" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="H131" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="H197" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="H241" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="H186" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="H187" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="H189" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="H336" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="H337" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="H344" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="H288" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="H277" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="H171" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="H147" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="H146" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="H116" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="H65" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="H54" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="H179" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId83"/>

</xml_diff>